<commit_message>
Updated with the new constant types fc_  function constant.
</commit_message>
<xml_diff>
--- a/SOURCE/PXI/DOC/Promax Interface Format 20130802_3.xlsx
+++ b/SOURCE/PXI/DOC/Promax Interface Format 20130802_3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="0" windowWidth="20730" windowHeight="4245" tabRatio="635" firstSheet="7" activeTab="10"/>
@@ -40,7 +40,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="14">'FFLU PMXPXI03 - 359PROM'!$A$1:$J$40</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="10">'PXIATL02 - CISATL14'!$A$1:$L$19</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -1385,8 +1385,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1562,7 +1562,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1597,7 +1596,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1773,7 +1771,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1781,7 +1779,7 @@
       <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1799,7 +1797,7 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>194</v>
       </c>
@@ -1828,7 +1826,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1857,7 +1855,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1886,7 +1884,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1915,7 +1913,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1944,7 +1942,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1973,7 +1971,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2002,7 +2000,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2025,7 +2023,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2054,7 +2052,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2080,7 +2078,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2103,7 +2101,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2129,7 +2127,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2158,7 +2156,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2184,7 +2182,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2210,7 +2208,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2251,7 +2249,7 @@
         <v>site_app.pmxpxi03_loader</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2280,7 +2278,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2321,7 +2319,7 @@
         <v>site_app.pmxpxi01_loader</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2350,7 +2348,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2391,7 +2389,7 @@
         <v>site_app.pmxpxi02_loader</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2420,7 +2418,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2449,7 +2447,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2478,7 +2476,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2515,7 +2513,7 @@
         <v>Promax NZ &gt; DFN : Demand : 337 : 337EST</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2541,7 +2539,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2561,7 +2559,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2581,17 +2579,17 @@
         <v>198</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="B28" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="B29" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="B30" s="1" t="s">
         <v>237</v>
       </c>
@@ -2603,7 +2601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -2613,10 +2611,10 @@
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -2637,7 +2635,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -2676,7 +2674,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="C2" s="1" t="s">
         <v>73</v>
       </c>
@@ -2703,11 +2701,11 @@
         <v/>
       </c>
       <c r="O2" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
-        <v>pxi_common.char_format('336002', 6, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '336002' -&gt; RecordType</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
+        <v>pxi_common.char_format('336002', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '336002' -&gt; RecordType</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -2735,11 +2733,11 @@
         <v/>
       </c>
       <c r="O3" s="8" t="str">
-        <f t="shared" ref="O3:O11" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O3:O11" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -2768,10 +2766,10 @@
       </c>
       <c r="O4" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>169</v>
       </c>
@@ -2800,10 +2798,10 @@
       </c>
       <c r="O5" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(invoicenumber, 10, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- invoicenumber -&gt; InvoiceNumber</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(invoicenumber, 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- invoicenumber -&gt; InvoiceNumber</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>170</v>
       </c>
@@ -2832,10 +2830,10 @@
       </c>
       <c r="O6" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(invoicelinenumber, 6, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- invoicelinenumber -&gt; InvoiceLineNumber</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(invoicelinenumber, 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- invoicelinenumber -&gt; InvoiceLineNumber</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>171</v>
       </c>
@@ -2868,10 +2866,10 @@
       </c>
       <c r="O7" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(customerhierarchy, 8, pxi_common.format_type_ltrim_zeros, pxi_common.is_not_nullable) || -- customerhierarchy -&gt; CustomerHierarchy</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(customerhierarchy, 8, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- customerhierarchy -&gt; CustomerHierarchy</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>172</v>
       </c>
@@ -2904,10 +2902,10 @@
       </c>
       <c r="O8" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(material, 18, pxi_common.format_type_ltrim_zeros, pxi_common.is_not_nullable) || -- material -&gt; Material</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(material, 18, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- material -&gt; Material</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>173</v>
       </c>
@@ -2939,10 +2937,10 @@
       </c>
       <c r="O9" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.date_format(invoicedate, 'yyyymmdd', pxi_common.is_not_nullable) || -- invoicedate -&gt; InvoiceDate</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.date_format(invoicedate, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- invoicedate -&gt; InvoiceDate</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
         <v>174</v>
       </c>
@@ -2974,10 +2972,10 @@
       </c>
       <c r="O10" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.numb_format(discountgiven, '9999990.00', pxi_common.is_not_nullable) || -- discountgiven -&gt; DiscountGiven</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.numb_format(discountgiven, '9999990.00', pxi_common.fc_is_not_nullable) || -- discountgiven -&gt; DiscountGiven</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>175</v>
       </c>
@@ -3007,7 +3005,7 @@
       </c>
       <c r="O11" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(conditiontype, 10, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- conditiontype -&gt; ConditionType</v>
+        <v>pxi_common.char_format(conditiontype, 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- conditiontype -&gt; ConditionType</v>
       </c>
     </row>
   </sheetData>
@@ -3017,16 +3015,18 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -3047,7 +3047,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="C2" s="1" t="s">
         <v>406</v>
       </c>
@@ -3113,11 +3113,11 @@
         <v/>
       </c>
       <c r="O2" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
-        <v>pxi_common.char_format('A', 1, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT 'A' -&gt; UsageConditionCode</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
+        <v>pxi_common.char_format('A', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'A' -&gt; UsageConditionCode</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>407</v>
       </c>
@@ -3146,11 +3146,11 @@
         <v/>
       </c>
       <c r="O3" s="8" t="str">
-        <f t="shared" ref="O3:O19" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format(cndtn_table_ref, 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- cndtn_table_ref -&gt; CondTable</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O3:O19" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
+        <v>pxi_common.char_format(cndtn_table_ref, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- cndtn_table_ref -&gt; CondTable</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="C4" s="1" t="s">
         <v>409</v>
       </c>
@@ -3179,10 +3179,10 @@
       </c>
       <c r="O4" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format('V', 1, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT 'V' -&gt; Application</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format('V', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'V' -&gt; Application</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>411</v>
       </c>
@@ -3210,11 +3210,11 @@
         <v/>
       </c>
       <c r="O5" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G5,IF(I5="Yes","_CONSTANT","")))), "::source_field::", A5), "::target_field::", C5), "::position::", D5), "::length::", E5), "::format::", H5), "::constant::", J5), "::is_nullable::", IF(F5="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L5), "none", LOWER(L5))))</f>
-        <v>pxi_common.char_format(VAKEY, 50, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- VAKEY -&gt; VAKEY</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(VAKEY, 50, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- VAKEY -&gt; VAKEY</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>412</v>
       </c>
@@ -3243,10 +3243,10 @@
       </c>
       <c r="O6" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(px_company_code, 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- px_company_code -&gt; CompanyCode</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(px_company_code, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- px_company_code -&gt; CompanyCode</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>414</v>
       </c>
@@ -3276,10 +3276,10 @@
       </c>
       <c r="O7" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(cust_div_code, 2, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- cust_div_code -&gt; Division</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(cust_div_code, 2, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- cust_div_code -&gt; Division</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>416</v>
       </c>
@@ -3309,10 +3309,10 @@
       </c>
       <c r="O8" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(cust_hier, 10, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- cust_hier -&gt; Customer</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(cust_hier, 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- cust_hier -&gt; Customer</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>172</v>
       </c>
@@ -3342,10 +3342,10 @@
       </c>
       <c r="O9" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(material, 18, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- material -&gt; Material</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(material, 18, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- material -&gt; Material</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
         <v>418</v>
       </c>
@@ -3377,10 +3377,10 @@
       </c>
       <c r="O10" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.date_format(buy_start_date, 'yyyymmdd', pxi_common.is_not_nullable) || -- buy_start_date -&gt; ValidFrom</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.date_format(buy_start_date, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- buy_start_date -&gt; ValidFrom</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>420</v>
       </c>
@@ -3412,10 +3412,10 @@
       </c>
       <c r="O11" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.date_format(buy_stop_date, 'yyyymmdd', pxi_common.is_not_nullable) || -- buy_stop_date -&gt; ValidTo</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.date_format(buy_stop_date, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- buy_stop_date -&gt; ValidTo</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
         <v>422</v>
       </c>
@@ -3445,10 +3445,10 @@
       </c>
       <c r="O12" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(pricing_cndtn_code, 4, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- pricing_cndtn_code -&gt; Condition</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(pricing_cndtn_code, 4, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- pricing_cndtn_code -&gt; Condition</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
         <v>424</v>
       </c>
@@ -3480,10 +3480,10 @@
       </c>
       <c r="O13" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(condition_type_code, 1, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- condition_type_code -&gt; ConditionType</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(condition_type_code, 1, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- condition_type_code -&gt; ConditionType</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
         <v>425</v>
       </c>
@@ -3515,10 +3515,10 @@
       </c>
       <c r="O14" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.numb_format(rate, 's9999990.00', pxi_common.is_not_nullable) || -- rate -&gt; Rate</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.numb_format(rate, 's9999990.00', pxi_common.fc_is_not_nullable) || -- rate -&gt; Rate</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
         <v>427</v>
       </c>
@@ -3548,10 +3548,10 @@
       </c>
       <c r="O15" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(rate_unit, 5, pxi_common.format_type_none, pxi_common.is_nullable) || -- rate_unit -&gt; RateUnit</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(rate_unit, 5, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- rate_unit -&gt; RateUnit</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="C16" s="1" t="s">
         <v>79</v>
       </c>
@@ -3581,10 +3581,10 @@
       </c>
       <c r="O16" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format('EA', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT 'EA' -&gt; UOM</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format('EA', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'EA' -&gt; UOM</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="1" t="s">
         <v>430</v>
       </c>
@@ -3616,10 +3616,10 @@
       </c>
       <c r="O17" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(sales_deal, 10, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- sales_deal -&gt; PromoNum</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(sales_deal, 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- sales_deal -&gt; PromoNum</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="1" t="s">
         <v>432</v>
       </c>
@@ -3648,10 +3648,10 @@
       </c>
       <c r="O18" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(rate_multiplier, 5, pxi_common.format_type_none, pxi_common.is_nullable) || -- rate_multiplier -&gt; PriceUnit</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(rate_multiplier, 5, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- rate_multiplier -&gt; PriceUnit</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
         <v>434</v>
       </c>
@@ -3680,7 +3680,7 @@
       </c>
       <c r="O19" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(order_type_code, 4, pxi_common.format_type_none, pxi_common.is_nullable) || -- order_type_code -&gt; OrderType</v>
+        <v>pxi_common.char_format(order_type_code, 4, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- order_type_code -&gt; OrderType</v>
       </c>
     </row>
   </sheetData>
@@ -3690,7 +3690,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -3703,7 +3703,7 @@
       <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="8" bestFit="1" customWidth="1"/>
@@ -3722,7 +3722,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="11.25">
       <c r="A1" s="8" t="s">
         <v>275</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="11.25">
       <c r="A2" s="1" t="s">
         <v>283</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>rec_type varchar2(3 char),</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="11.25">
       <c r="A3" s="1" t="s">
         <v>285</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>idoc_type varchar2(30 char),</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="11.25">
       <c r="A4" s="1" t="s">
         <v>287</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>idoc_no number(16,0),</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="11.25">
       <c r="A5" s="1" t="s">
         <v>290</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>idoc_date date,</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="11.25">
       <c r="B6" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4066,7 +4066,7 @@
       </c>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="11.25">
       <c r="A7" s="1" t="s">
         <v>283</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>rec_type varchar2(3 char),</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="11.25">
       <c r="A8" s="1" t="s">
         <v>292</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>company_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="11.25">
       <c r="A9" s="1" t="s">
         <v>293</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>div_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="11.25">
       <c r="A10" s="1" t="s">
         <v>294</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>cust_code varchar2(10 char),</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="11.25">
       <c r="A11" s="1" t="s">
         <v>296</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>claim_amount number(15,4),</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="11.25">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -4383,7 +4383,7 @@
         <v>claim_ref varchar2(12 char),</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="11.25">
       <c r="A13" s="1" t="s">
         <v>301</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>assignment_no varchar2(18 char),</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="11.25">
       <c r="A14" s="1" t="s">
         <v>303</v>
       </c>
@@ -4484,7 +4484,7 @@
         <v>tax_base number(15,4),</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="11.25">
       <c r="A15" s="1" t="s">
         <v>304</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>posting_date date,</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="11.25">
       <c r="A16" s="1" t="s">
         <v>305</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>fiscal_period number(2,0),</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="11.25">
       <c r="A17" s="1" t="s">
         <v>308</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>reason_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="11.25">
       <c r="A18" s="1" t="s">
         <v>309</v>
       </c>
@@ -4687,7 +4687,7 @@
         <v>accounting_doc_no varchar2(10 char),</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="11.25">
       <c r="A19" s="1" t="s">
         <v>310</v>
       </c>
@@ -4739,7 +4739,7 @@
         <v>fiscal_year number(4,0),</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="11.25">
       <c r="A20" s="1" t="s">
         <v>313</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>line_item_no varchar2(3),</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="11.25">
       <c r="A21" s="1" t="s">
         <v>315</v>
       </c>
@@ -4838,7 +4838,7 @@
         <v>bus_partner_ref varchar2(12 char),</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="11.25">
       <c r="A22" s="1" t="s">
         <v>316</v>
       </c>
@@ -4887,43 +4887,43 @@
         <v>tax_code varchar2(2 char),</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="11.25">
       <c r="K23" s="8"/>
     </row>
-    <row r="24" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="11.25">
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="11.25">
       <c r="K25" s="8"/>
     </row>
-    <row r="26" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="11.25">
       <c r="K26" s="8"/>
     </row>
-    <row r="27" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="11.25">
       <c r="K27" s="8"/>
     </row>
-    <row r="28" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="11.25">
       <c r="K28" s="8"/>
     </row>
-    <row r="29" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="11.25">
       <c r="K29" s="8"/>
     </row>
-    <row r="30" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="11.25">
       <c r="K30" s="8"/>
     </row>
-    <row r="31" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="11.25">
       <c r="K31" s="8"/>
     </row>
-    <row r="32" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="11.25">
       <c r="K32" s="8"/>
     </row>
-    <row r="33" spans="11:11" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="11:11" s="1" customFormat="1" ht="11.25">
       <c r="K33" s="8"/>
     </row>
-    <row r="34" spans="11:11" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="11:11" s="1" customFormat="1" ht="11.25">
       <c r="K34" s="8"/>
     </row>
-    <row r="35" spans="11:11" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="11:11" s="1" customFormat="1" ht="11.25">
       <c r="K35" s="8"/>
     </row>
   </sheetData>
@@ -4932,7 +4932,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4945,7 +4945,7 @@
       <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="8" bestFit="1" customWidth="1"/>
@@ -4964,7 +4964,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="11.25">
       <c r="A1" s="8" t="s">
         <v>275</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="11.25">
       <c r="A2" s="1" t="s">
         <v>318</v>
       </c>
@@ -5077,7 +5077,7 @@
         <v>ic_record_type varchar2(6 char),</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="11.25">
       <c r="A3" s="1" t="s">
         <v>320</v>
       </c>
@@ -5147,7 +5147,7 @@
         <v>px_company_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="11.25">
       <c r="A4" s="1" t="s">
         <v>321</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>px_division_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="11.25">
       <c r="A5" s="1" t="s">
         <v>283</v>
       </c>
@@ -5245,7 +5245,7 @@
         <v>rec_type varchar2(1 char),</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="11.25">
       <c r="A6" s="1" t="s">
         <v>323</v>
       </c>
@@ -5297,7 +5297,7 @@
         <v>document_date date,</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="11.25">
       <c r="A7" s="1" t="s">
         <v>304</v>
       </c>
@@ -5349,7 +5349,7 @@
         <v>posting_date date,</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="11.25">
       <c r="A8" s="1" t="s">
         <v>324</v>
       </c>
@@ -5398,7 +5398,7 @@
         <v>document_type varchar2(2 char),</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="11.25">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -5447,7 +5447,7 @@
         <v>currency varchar2(3 char),</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="11.25">
       <c r="A10" s="1" t="s">
         <v>141</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>reference varchar2(16 char),</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="11.25">
       <c r="A11" s="1" t="s">
         <v>326</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>document_header_text varchar2(25 char),</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="11.25">
       <c r="A12" s="1" t="s">
         <v>328</v>
       </c>
@@ -5594,7 +5594,7 @@
         <v>posting_key varchar2(4 char),</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="11.25">
       <c r="A13" s="1" t="s">
         <v>179</v>
       </c>
@@ -5643,7 +5643,7 @@
         <v>account varchar2(17 char),</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="11.25">
       <c r="A14" s="1" t="s">
         <v>331</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>pa_assignment_flag varchar2(1 char),</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="11.25">
       <c r="A15" s="1" t="s">
         <v>148</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>amount number(13,2),</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="11.25">
       <c r="A16" s="1" t="s">
         <v>332</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>payment_method varchar2(1 char),</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="11.25">
       <c r="A17" s="1" t="s">
         <v>181</v>
       </c>
@@ -5842,7 +5842,7 @@
         <v>allocation varchar2(18 char),</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="11.25">
       <c r="A18" s="1" t="s">
         <v>182</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>text varchar2(30 char),</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="11.25">
       <c r="A19" s="1" t="s">
         <v>333</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>profit_centre varchar2(10 char),</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="11.25">
       <c r="A20" s="1" t="s">
         <v>334</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>cost_centre varchar2(10 char),</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="11.25">
       <c r="A21" s="1" t="s">
         <v>335</v>
       </c>
@@ -6038,7 +6038,7 @@
         <v>sales_organisation varchar2(4 char),</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="11.25">
       <c r="A22" s="1" t="s">
         <v>336</v>
       </c>
@@ -6087,7 +6087,7 @@
         <v>sales_office varchar2(5 char),</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="11.25">
       <c r="A23" s="1" t="s">
         <v>338</v>
       </c>
@@ -6136,7 +6136,7 @@
         <v>product_number varchar2(18 char),</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="11.25">
       <c r="A24" s="1" t="s">
         <v>339</v>
       </c>
@@ -6185,7 +6185,7 @@
         <v>pa_code varchar2(5 char),</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="11.25">
       <c r="A25" s="1" t="s">
         <v>340</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>glt_row_id varchar2(10 char),</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="11.25">
       <c r="A26" s="1" t="s">
         <v>341</v>
       </c>
@@ -6283,7 +6283,7 @@
         <v>user_1 varchar2(10 char),</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="11.25">
       <c r="A27" s="1" t="s">
         <v>342</v>
       </c>
@@ -6332,7 +6332,7 @@
         <v>user_2 varchar2(10 char),</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="11.25">
       <c r="A28" s="1" t="s">
         <v>343</v>
       </c>
@@ -6384,7 +6384,7 @@
         <v>buy_start_date date,</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="11.25">
       <c r="A29" s="1" t="s">
         <v>344</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>buy_stop_date date,</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="11.25">
       <c r="A30" s="1" t="s">
         <v>345</v>
       </c>
@@ -6488,7 +6488,7 @@
         <v>start_date date,</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="11.25">
       <c r="A31" s="1" t="s">
         <v>346</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>stop_date date,</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="11.25">
       <c r="A32" s="1" t="s">
         <v>183</v>
       </c>
@@ -6589,7 +6589,7 @@
         <v>quantity varchar2(15 char),</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="11.25">
       <c r="A33" s="1" t="s">
         <v>348</v>
       </c>
@@ -6638,7 +6638,7 @@
         <v>additional_info varchar2(10 char),</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="11.25">
       <c r="A34" s="1" t="s">
         <v>349</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>promotion_is_closed varchar2(1 char),</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="11.25">
       <c r="K35" s="8"/>
     </row>
   </sheetData>
@@ -6696,7 +6696,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6709,7 +6709,7 @@
       <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" style="16" bestFit="1" customWidth="1"/>
@@ -6728,7 +6728,7 @@
     <col min="15" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="16" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="16" customFormat="1" ht="11.25">
       <c r="A1" s="16" t="s">
         <v>275</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="11.25">
       <c r="A2" s="17" t="s">
         <v>318</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>ic_record_type varchar2(6 char),</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="11.25">
       <c r="A3" s="17" t="s">
         <v>320</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>px_company_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="11.25">
       <c r="A4" s="17" t="s">
         <v>321</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>px_division_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="11.25">
       <c r="A5" s="17" t="s">
         <v>8</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>type varchar2(1 char),</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="11.25">
       <c r="A6" s="17" t="s">
         <v>323</v>
       </c>
@@ -7054,7 +7054,7 @@
         <v>document_date date,</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="11.25">
       <c r="A7" s="17" t="s">
         <v>304</v>
       </c>
@@ -7106,7 +7106,7 @@
         <v>posting_date date,</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="11.25">
       <c r="A8" s="17" t="s">
         <v>350</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>claim_date date,</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="11.25">
       <c r="A9" s="17" t="s">
         <v>141</v>
       </c>
@@ -7207,7 +7207,7 @@
         <v>reference varchar2(10 char),</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="11.25">
       <c r="A10" s="17" t="s">
         <v>326</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>document_header_text varchar2(25 char),</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="11.25">
       <c r="A11" s="17" t="s">
         <v>351</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>expenditure_type varchar2(5 char),</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="11.25">
       <c r="A12" s="17" t="s">
         <v>328</v>
       </c>
@@ -7354,7 +7354,7 @@
         <v>posting_key varchar2(7 char),</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="11.25">
       <c r="A13" s="17" t="s">
         <v>353</v>
       </c>
@@ -7403,7 +7403,7 @@
         <v>account_code varchar2(10 char),</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="11.25">
       <c r="A14" s="17" t="s">
         <v>148</v>
       </c>
@@ -7455,7 +7455,7 @@
         <v>amount number(14,2),</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="11.25">
       <c r="A15" s="17" t="s">
         <v>354</v>
       </c>
@@ -7507,7 +7507,7 @@
         <v>spend_amount number(14,2),</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="11.25">
       <c r="A16" s="17" t="s">
         <v>355</v>
       </c>
@@ -7559,7 +7559,7 @@
         <v>tax_amount number(14,2),</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="11.25">
       <c r="A17" s="17" t="s">
         <v>332</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>payment_method varchar2(1 char),</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="11.25">
       <c r="A18" s="17" t="s">
         <v>181</v>
       </c>
@@ -7657,7 +7657,7 @@
         <v>allocation varchar2(12 char),</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="11.25">
       <c r="A19" s="17" t="s">
         <v>356</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>pc_reference varchar2(18 char),</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="11.25">
       <c r="A20" s="17" t="s">
         <v>357</v>
       </c>
@@ -7755,7 +7755,7 @@
         <v>px_reference varchar2(60 char),</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="11.25">
       <c r="A21" s="17" t="s">
         <v>359</v>
       </c>
@@ -7804,7 +7804,7 @@
         <v>ext_reference varchar2(65 char),</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="11.25">
       <c r="A22" s="17" t="s">
         <v>338</v>
       </c>
@@ -7853,7 +7853,7 @@
         <v>product_number varchar2(18 char),</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="11.25">
       <c r="A23" s="17" t="s">
         <v>361</v>
       </c>
@@ -7902,7 +7902,7 @@
         <v>transaction_code varchar2(40 char),</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="11.25">
       <c r="A24" s="17" t="s">
         <v>363</v>
       </c>
@@ -7951,7 +7951,7 @@
         <v>deduction_ac_code varchar2(20 char),</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="11.25">
       <c r="A25" s="17" t="s">
         <v>365</v>
       </c>
@@ -8000,7 +8000,7 @@
         <v>payee_code varchar2(10 char),</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="11.25">
       <c r="A26" s="17" t="s">
         <v>366</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>debit_code varchar2(20 char),</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="11.25">
       <c r="A27" s="17" t="s">
         <v>367</v>
       </c>
@@ -8098,7 +8098,7 @@
         <v>credit_code varchar2(20 char),</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="11.25">
       <c r="A28" s="17" t="s">
         <v>368</v>
       </c>
@@ -8147,7 +8147,7 @@
         <v>customer_is_a_vendor varchar2(1 char),</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="11.25">
       <c r="A29" s="17" t="s">
         <v>39</v>
       </c>
@@ -8196,7 +8196,7 @@
         <v>currency varchar2(3 char),</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="11.25">
       <c r="A30" s="17" t="s">
         <v>369</v>
       </c>
@@ -8245,7 +8245,7 @@
         <v>promo_claim_detail_row_id varchar2(10 char),</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="11.25">
       <c r="A31" s="17" t="s">
         <v>370</v>
       </c>
@@ -8294,7 +8294,7 @@
         <v>promo_claim_group_row_id varchar2(10 char),</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="11.25">
       <c r="A32" s="17" t="s">
         <v>371</v>
       </c>
@@ -8343,7 +8343,7 @@
         <v>promo_claim_group_pub_id varchar2(30 char),</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="11.25">
       <c r="A33" s="17" t="s">
         <v>308</v>
       </c>
@@ -8392,7 +8392,7 @@
         <v>reason_code varchar2(5 char),</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="11.25">
       <c r="A34" s="17" t="s">
         <v>372</v>
       </c>
@@ -8441,7 +8441,7 @@
         <v>pc_message varchar2(65 char),</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="11.25">
       <c r="A35" s="17" t="s">
         <v>373</v>
       </c>
@@ -8490,7 +8490,7 @@
         <v>pc_comment varchar2(200 char),</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="11.25">
       <c r="A36" s="17" t="s">
         <v>375</v>
       </c>
@@ -8539,7 +8539,7 @@
         <v>text_1 varchar2(40 char),</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="11.25">
       <c r="A37" s="17" t="s">
         <v>376</v>
       </c>
@@ -8588,7 +8588,7 @@
         <v>text_2 varchar2(40 char),</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="11.25">
       <c r="A38" s="17" t="s">
         <v>343</v>
       </c>
@@ -8640,7 +8640,7 @@
         <v>buy_start_date date,</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="11.25">
       <c r="A39" s="17" t="s">
         <v>344</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>buy_stop_date date,</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="11.25">
       <c r="A40" s="17" t="s">
         <v>377</v>
       </c>
@@ -8747,7 +8747,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
@@ -8761,7 +8761,7 @@
       <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="8" bestFit="1" customWidth="1"/>
@@ -8780,7 +8780,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="11.25">
       <c r="A1" s="8" t="s">
         <v>275</v>
       </c>
@@ -8824,7 +8824,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="11.25">
       <c r="A2" s="1" t="s">
         <v>318</v>
       </c>
@@ -8893,7 +8893,7 @@
         <v>ic_record_type varchar2(6 char),</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="11.25">
       <c r="A3" s="1" t="s">
         <v>320</v>
       </c>
@@ -8956,7 +8956,7 @@
         <v>px_company_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="11.25">
       <c r="A4" s="1" t="s">
         <v>321</v>
       </c>
@@ -9005,7 +9005,7 @@
         <v>px_division_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="11.25">
       <c r="A5" s="1" t="s">
         <v>210</v>
       </c>
@@ -9054,7 +9054,7 @@
         <v>customer_hierarchy varchar2(10 char),</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="11.25">
       <c r="A6" s="1" t="s">
         <v>378</v>
       </c>
@@ -9103,7 +9103,7 @@
         <v>sales_deal varchar2(10 char),</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="11.25">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -9152,7 +9152,7 @@
         <v>material varchar2(18 char),</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="11.25">
       <c r="A8" s="1" t="s">
         <v>343</v>
       </c>
@@ -9204,7 +9204,7 @@
         <v>buy_start_date date,</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="11.25">
       <c r="A9" s="1" t="s">
         <v>344</v>
       </c>
@@ -9256,7 +9256,7 @@
         <v>buy_stop_date date,</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="11.25">
       <c r="A10" s="1" t="s">
         <v>361</v>
       </c>
@@ -9305,7 +9305,7 @@
         <v>transaction_code varchar2(4 char),</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="11.25">
       <c r="A11" s="1" t="s">
         <v>109</v>
       </c>
@@ -9354,7 +9354,7 @@
         <v>description varchar2(40 char),</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="11.25">
       <c r="A12" s="1" t="s">
         <v>379</v>
       </c>
@@ -9403,7 +9403,7 @@
         <v>sales_org varchar2(4 char),</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="11.25">
       <c r="A13" s="1" t="s">
         <v>176</v>
       </c>
@@ -9455,7 +9455,7 @@
         <v>rate number(12,2),</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="11.25">
       <c r="A14" s="1" t="s">
         <v>341</v>
       </c>
@@ -9504,7 +9504,7 @@
         <v>user_1 varchar2(10 char),</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="11.25">
       <c r="A15" s="1" t="s">
         <v>342</v>
       </c>
@@ -9553,7 +9553,7 @@
         <v>user_2 varchar2(10 char),</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="11.25">
       <c r="A16" s="1" t="s">
         <v>380</v>
       </c>
@@ -9602,7 +9602,7 @@
         <v>action_code varchar2(1 char),</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="11.25">
       <c r="A17" s="1" t="s">
         <v>381</v>
       </c>
@@ -9651,7 +9651,7 @@
         <v>bonus_stock_description varchar2(100 char),</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="11.25">
       <c r="A18" s="1" t="s">
         <v>383</v>
       </c>
@@ -9703,7 +9703,7 @@
         <v>bonus_stock_hurdle number(9,2),</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="11.25">
       <c r="A19" s="1" t="s">
         <v>384</v>
       </c>
@@ -9755,7 +9755,7 @@
         <v>bonus_stock_receive number(9,2),</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="11.25">
       <c r="A20" s="1" t="s">
         <v>385</v>
       </c>
@@ -9804,7 +9804,7 @@
         <v>bonus_stock_sku_code varchar2(18 char),</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="11.25">
       <c r="A21" s="1" t="s">
         <v>386</v>
       </c>
@@ -9853,7 +9853,7 @@
         <v>rate_unit varchar2(5 char),</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="11.25">
       <c r="A22" s="1" t="s">
         <v>387</v>
       </c>
@@ -9902,7 +9902,7 @@
         <v>condition_pricing_unit varchar2(5 char),</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="11.25">
       <c r="A23" s="1" t="s">
         <v>388</v>
       </c>
@@ -9951,7 +9951,7 @@
         <v>condition_uom varchar2(3 char),</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="11.25">
       <c r="A24" s="1" t="s">
         <v>389</v>
       </c>
@@ -10000,7 +10000,7 @@
         <v>sap_promo_number varchar2(10 char),</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="11.25">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
@@ -10049,7 +10049,7 @@
         <v>currency varchar2(3 char),</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="11.25">
       <c r="A26" s="1" t="s">
         <v>390</v>
       </c>
@@ -10098,7 +10098,7 @@
         <v>uom_str_unit varchar2(3 char),</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="11.25">
       <c r="A27" s="1" t="s">
         <v>391</v>
       </c>
@@ -10147,7 +10147,7 @@
         <v>uom_str_saleable varchar2(3 char),</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="11.25">
       <c r="A28" s="1" t="s">
         <v>392</v>
       </c>
@@ -10196,7 +10196,7 @@
         <v>promo_price_saleable varchar2(10 char),</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="11.25">
       <c r="A29" s="1" t="s">
         <v>393</v>
       </c>
@@ -10245,7 +10245,7 @@
         <v>promo_price_unit varchar2(10 char),</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="11.25">
       <c r="A30" s="1" t="s">
         <v>394</v>
       </c>
@@ -10294,7 +10294,7 @@
         <v>transaction_amount varchar2(10 char),</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="11.25">
       <c r="A31" s="1" t="s">
         <v>395</v>
       </c>
@@ -10343,14 +10343,14 @@
         <v>payer_code varchar2(20 char),</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="11.25">
       <c r="I32" s="7" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K32" s="8"/>
     </row>
-    <row r="33" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="11.25">
       <c r="A33" s="1" t="s">
         <v>436</v>
       </c>
@@ -10396,7 +10396,7 @@
         <v>condition_flag varchar2(1 char),</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="11.25">
       <c r="A34" s="1" t="s">
         <v>437</v>
       </c>
@@ -10442,7 +10442,7 @@
         <v>business_segment varchar2(2 char),</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="11.25">
       <c r="A35" s="1" t="s">
         <v>438</v>
       </c>
@@ -10488,7 +10488,7 @@
         <v>rate_multiplier number(4),</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="11.25">
       <c r="A36" s="1" t="s">
         <v>440</v>
       </c>
@@ -10534,7 +10534,7 @@
         <v>condition_type_code varchar2(1 char),</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="11.25">
       <c r="A37" s="1" t="s">
         <v>441</v>
       </c>
@@ -10580,7 +10580,7 @@
         <v>pricing_condition_code varchar2(4 char),</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="11.25">
       <c r="A38" s="1" t="s">
         <v>442</v>
       </c>
@@ -10626,7 +10626,7 @@
         <v>condition_table_ref varchar2(5 char),</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="11.25">
       <c r="A39" s="1" t="s">
         <v>443</v>
       </c>
@@ -10672,7 +10672,7 @@
         <v>cust_div_code varchar2(2 char),</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="11.25">
       <c r="A40" s="1" t="s">
         <v>444</v>
       </c>
@@ -10725,7 +10725,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10733,17 +10733,17 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="130.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -10751,15 +10751,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" s="13" customFormat="1">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" s="6" customFormat="1">
       <c r="A3" s="6" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
@@ -10767,7 +10767,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="8" t="s">
         <v>23</v>
       </c>
@@ -10775,7 +10775,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
@@ -10783,7 +10783,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -10791,7 +10791,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="6" t="s">
         <v>72</v>
       </c>
@@ -10799,32 +10799,32 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="B10" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="B11" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2">
       <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2">
       <c r="B13" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" s="8" customFormat="1">
       <c r="A15" s="6" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2">
       <c r="A16" s="8" t="s">
         <v>259</v>
       </c>
@@ -10832,7 +10832,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2">
       <c r="A17" s="8" t="s">
         <v>261</v>
       </c>
@@ -10840,7 +10840,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2">
       <c r="A18" s="8" t="s">
         <v>263</v>
       </c>
@@ -10848,7 +10848,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2">
       <c r="A20" s="8" t="s">
         <v>265</v>
       </c>
@@ -10856,7 +10856,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2">
       <c r="A21" s="8" t="s">
         <v>267</v>
       </c>
@@ -10864,7 +10864,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2">
       <c r="A22" s="8" t="s">
         <v>269</v>
       </c>
@@ -10872,7 +10872,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2">
       <c r="A24" s="8" t="s">
         <v>271</v>
       </c>
@@ -10887,20 +10887,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D33" sqref="D33"/>
+      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -10921,7 +10921,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -10960,7 +10960,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="C2" s="1" t="s">
         <v>73</v>
       </c>
@@ -10987,11 +10987,11 @@
         <v/>
       </c>
       <c r="O2" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
-        <v>pxi_common.char_format('302001', 6, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '302001' -&gt; RecordType</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
+        <v>pxi_common.char_format('302001', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '302001' -&gt; RecordType</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -11020,11 +11020,11 @@
         <v/>
       </c>
       <c r="O3" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O3:O22" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -11053,11 +11053,11 @@
         <v/>
       </c>
       <c r="O4" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G4,IF(I4="Yes","_CONSTANT","")))), "::source_field::", A4), "::target_field::", C4), "::position::", D4), "::length::", E4), "::format::", H4), "::constant::", J4), "::is_nullable::", IF(F4="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L4), "none", LOWER(L4))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>92</v>
       </c>
@@ -11084,15 +11084,15 @@
         <v>64</v>
       </c>
       <c r="M5" s="7" t="str">
-        <f t="shared" ref="M5:M20" si="2">IF(ISBLANK(H5),"",CONCATENATE(IF(LEN(H5)&lt;&gt;E5,"#",""),LEN(H5)))</f>
+        <f t="shared" ref="M5:M20" si="3">IF(ISBLANK(H5),"",CONCATENATE(IF(LEN(H5)&lt;&gt;E5,"#",""),LEN(H5)))</f>
         <v/>
       </c>
       <c r="O5" s="8" t="str">
-        <f t="shared" ref="O5:O20" ca="1" si="3">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G5,IF(I5="Yes","_CONSTANT","")))), "::source_field::", A5), "::target_field::", C5), "::position::", D5), "::length::", E5), "::format::", H5), "::constant::", J5), "::is_nullable::", IF(F5="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L5), "none", LOWER(L5))))</f>
-        <v>pxi_common.char_format(zrep_matl_code, 18, pxi_common.format_type_ltrim_zeros, pxi_common.is_not_nullable) || -- zrep_matl_code -&gt; ProductItemNumber</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(zrep_matl_code, 18, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- zrep_matl_code -&gt; ProductItemNumber</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>93</v>
       </c>
@@ -11116,15 +11116,15 @@
         <v>0</v>
       </c>
       <c r="M6" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O6" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format(zrep_matl_desc, 40, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- zrep_matl_desc -&gt; Description</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(zrep_matl_desc, 40, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- zrep_matl_desc -&gt; Description</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="C7" s="1" t="s">
         <v>75</v>
       </c>
@@ -11148,15 +11148,15 @@
         <v>106</v>
       </c>
       <c r="M7" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O7" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format('1', 2, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '1' -&gt; Status</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format('1', 2, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '1' -&gt; Status</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>92</v>
       </c>
@@ -11183,15 +11183,15 @@
         <v>64</v>
       </c>
       <c r="M8" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O8" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format(zrep_matl_code, 10, pxi_common.format_type_ltrim_zeros, pxi_common.is_nullable) || -- zrep_matl_code -&gt; ShortName</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(zrep_matl_code, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_nullable) || -- zrep_matl_code -&gt; ShortName</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>94</v>
       </c>
@@ -11215,15 +11215,15 @@
         <v>0</v>
       </c>
       <c r="M9" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O9" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format(rsu_ean, 18, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- rsu_ean -&gt; APN</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(rsu_ean, 18, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- rsu_ean -&gt; APN</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
         <v>95</v>
       </c>
@@ -11247,15 +11247,15 @@
         <v>0</v>
       </c>
       <c r="M10" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O10" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format(tdu_ean, 18, pxi_common.format_type_none, pxi_common.is_nullable) || -- tdu_ean -&gt; TUN</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(tdu_ean, 18, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- tdu_ean -&gt; TUN</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>110</v>
       </c>
@@ -11279,15 +11279,15 @@
         <v>0</v>
       </c>
       <c r="M11" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O11" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format(rsu_uom, 3, pxi_common.format_type_none, pxi_common.is_nullable) || -- rsu_uom -&gt; UOM</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(rsu_uom, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- rsu_uom -&gt; UOM</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
         <v>96</v>
       </c>
@@ -11312,15 +11312,15 @@
         <v>0</v>
       </c>
       <c r="M12" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O12" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format(tdu_uom, 3, pxi_common.format_type_none, pxi_common.is_nullable) || -- tdu_uom -&gt; SellableUOM</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(tdu_uom, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- tdu_uom -&gt; SellableUOM</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
         <v>104</v>
       </c>
@@ -11347,15 +11347,15 @@
         <v>0</v>
       </c>
       <c r="M13" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="O13" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.numb_format(rsus_per_tdu, '99999999999990', pxi_common.is_nullable) || -- rsus_per_tdu -&gt; UnitsPerCase</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.numb_format(rsus_per_tdu, '99999999999990', pxi_common.fc_is_nullable) || -- rsus_per_tdu -&gt; UnitsPerCase</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
         <v>104</v>
       </c>
@@ -11382,15 +11382,15 @@
         <v>0</v>
       </c>
       <c r="M14" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="O14" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.numb_format(rsus_per_tdu, '99999999999990', pxi_common.is_nullable) || -- rsus_per_tdu -&gt; BaseUnitsPerSellable</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.numb_format(rsus_per_tdu, '99999999999990', pxi_common.fc_is_nullable) || -- rsus_per_tdu -&gt; BaseUnitsPerSellable</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
@@ -11414,15 +11414,15 @@
         <v>108</v>
       </c>
       <c r="M15" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O15" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G15,IF(I15="Yes","_CONSTANT","")))), "::source_field::", A15), "::target_field::", C15), "::position::", D15), "::length::", E15), "::format::", H15), "::constant::", J15), "::is_nullable::", IF(F15="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L15), "none", LOWER(L15))))</f>
-        <v>pxi_common.char_format('0', 1, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '0' -&gt; Type</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format('0', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '0' -&gt; Type</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
         <v>103</v>
       </c>
@@ -11449,15 +11449,15 @@
         <v>0</v>
       </c>
       <c r="M16" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="O16" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.numb_format(tdu_net_weight, '9999999990.000', pxi_common.is_nullable) || -- tdu_net_weight -&gt; ShipperNetWeightKG</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.numb_format(tdu_net_weight, '9999999990.000', pxi_common.fc_is_nullable) || -- tdu_net_weight -&gt; ShipperNetWeightKG</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="1" t="s">
         <v>99</v>
       </c>
@@ -11484,15 +11484,15 @@
         <v>0</v>
       </c>
       <c r="M17" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="O17" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.numb_format(tdu_height, '9999999990', pxi_common.is_nullable) || -- tdu_height -&gt; CaseHeight</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.numb_format(tdu_height, '9999999990', pxi_common.fc_is_nullable) || -- tdu_height -&gt; CaseHeight</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="1" t="s">
         <v>98</v>
       </c>
@@ -11519,15 +11519,15 @@
         <v>0</v>
       </c>
       <c r="M18" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="O18" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G18,IF(I18="Yes","_CONSTANT","")))), "::source_field::", A18), "::target_field::", C18), "::position::", D18), "::length::", E18), "::format::", H18), "::constant::", J18), "::is_nullable::", IF(F18="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L18), "none", LOWER(L18))))</f>
-        <v>pxi_common.numb_format(tdu_width, '9999999990', pxi_common.is_nullable) || -- tdu_width -&gt; CaseWidth</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.numb_format(tdu_width, '9999999990', pxi_common.fc_is_nullable) || -- tdu_width -&gt; CaseWidth</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
         <v>97</v>
       </c>
@@ -11554,15 +11554,15 @@
         <v>0</v>
       </c>
       <c r="M19" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="O19" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.numb_format(tdu_length, '9999999990', pxi_common.is_nullable) || -- tdu_length -&gt; CaseLength</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.numb_format(tdu_length, '9999999990', pxi_common.fc_is_nullable) || -- tdu_length -&gt; CaseLength</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="1" t="s">
         <v>100</v>
       </c>
@@ -11589,15 +11589,15 @@
         <v>0</v>
       </c>
       <c r="M20" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="O20" s="8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.numb_format(rsu_height, '9999999990', pxi_common.is_nullable) || -- rsu_height -&gt; UnitHeight</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.numb_format(rsu_height, '9999999990', pxi_common.fc_is_nullable) || -- rsu_height -&gt; UnitHeight</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="1" t="s">
         <v>101</v>
       </c>
@@ -11628,11 +11628,11 @@
         <v>10</v>
       </c>
       <c r="O21" s="8" t="str">
-        <f t="shared" ref="O21:O22" ca="1" si="5">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G21,IF(I21="Yes","_CONSTANT","")))), "::source_field::", A21), "::target_field::", C21), "::position::", D21), "::length::", E21), "::format::", H21), "::constant::", J21), "::is_nullable::", IF(F21="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L21), "none", LOWER(L21))))</f>
-        <v>pxi_common.numb_format(rsu_width, '9999999990', pxi_common.is_nullable) || -- rsu_width -&gt; UnitWidth</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.numb_format(rsu_width, '9999999990', pxi_common.fc_is_nullable) || -- rsu_width -&gt; UnitWidth</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="1" t="s">
         <v>102</v>
       </c>
@@ -11663,8 +11663,8 @@
         <v>10</v>
       </c>
       <c r="O22" s="8" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>pxi_common.numb_format(rsu_length, '9999999990', pxi_common.is_nullable) || -- rsu_length -&gt; UnitLength</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.numb_format(rsu_length, '9999999990', pxi_common.fc_is_nullable) || -- rsu_length -&gt; UnitLength</v>
       </c>
     </row>
   </sheetData>
@@ -11674,20 +11674,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2:O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -11708,7 +11708,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -11747,7 +11747,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -11774,16 +11774,16 @@
         <v/>
       </c>
       <c r="O2" s="8" t="str">
-        <f t="shared" ref="O2:O8" ca="1" si="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
-        <v>pxi_common.char_format('303002', 6, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '303002' -&gt; ICRecordType</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
+        <v>pxi_common.char_format('303002', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '303002' -&gt; ICRecordType</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3:D4" si="2">D2+E2</f>
+        <f t="shared" ref="D3:D4" si="1">D2+E2</f>
         <v>6</v>
       </c>
       <c r="E3" s="1">
@@ -11806,16 +11806,16 @@
         <v/>
       </c>
       <c r="O3" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O3:O8" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E4" s="1">
@@ -11838,11 +11838,11 @@
         <v/>
       </c>
       <c r="O4" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
@@ -11874,11 +11874,11 @@
         <v/>
       </c>
       <c r="O5" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format(node_code, 40, pxi_common.format_type_ltrim_zeros, pxi_common.is_not_nullable) || -- node_code -&gt; Attribute</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(node_code, 40, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- node_code -&gt; Attribute</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>132</v>
       </c>
@@ -11906,11 +11906,11 @@
         <v/>
       </c>
       <c r="O6" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format(node_name, 40, pxi_common.format_type_none, pxi_common.is_nullable) || -- node_name -&gt; NodeName</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(node_name, 40, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- node_name -&gt; NodeName</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>133</v>
       </c>
@@ -11941,11 +11941,11 @@
         <v/>
       </c>
       <c r="O7" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format(parent_node_code, 40, pxi_common.format_type_ltrim_zeros, pxi_common.is_nullable) || -- parent_node_code -&gt; ParrentAttribute</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(parent_node_code, 40, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_nullable) || -- parent_node_code -&gt; ParrentAttribute</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>134</v>
       </c>
@@ -11976,55 +11976,55 @@
         <v/>
       </c>
       <c r="O8" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format(material_code, 18, pxi_common.format_type_ltrim_zeros, pxi_common.is_nullable) || -- material_code -&gt; MaterialNumber</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(material_code, 18, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_nullable) || -- material_code -&gt; MaterialNumber</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="M9" s="7" t="str">
         <f>IF(ISBLANK(H9),"",CONCATENATE(IF(LEN(H9)&lt;&gt;E9,"#",""),LEN(H9)))</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="J10" s="10"/>
       <c r="M10" s="7" t="str">
         <f t="shared" ref="M10:M13" si="4">IF(ISBLANK(H10),"",CONCATENATE(IF(LEN(H10)&lt;&gt;E10,"#",""),LEN(H10)))</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15">
       <c r="M11" s="7" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="M12" s="7" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15">
       <c r="M13" s="7" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="10:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="10:15" ht="15">
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="10:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="10:15" ht="15">
       <c r="J23" s="10"/>
       <c r="O23" s="9"/>
     </row>
-    <row r="24" spans="10:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="10:15" ht="15">
       <c r="O24" s="9"/>
     </row>
-    <row r="25" spans="10:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="10:15" ht="15">
       <c r="O25" s="9"/>
     </row>
-    <row r="26" spans="10:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="10:15" ht="15">
       <c r="O26" s="9"/>
     </row>
   </sheetData>
@@ -12034,20 +12034,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -12068,7 +12068,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -12107,7 +12107,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="C2" s="1" t="s">
         <v>73</v>
       </c>
@@ -12134,11 +12134,11 @@
         <v/>
       </c>
       <c r="O2" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
-        <v>pxi_common.char_format('300001', 6, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '300001' -&gt; RecordType</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
+        <v>pxi_common.char_format('300001', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '300001' -&gt; RecordType</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
@@ -12166,11 +12166,11 @@
         <v/>
       </c>
       <c r="O3" s="8" t="str">
-        <f t="shared" ref="O3:O4" ca="1" si="3">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O3:O11" ca="1" si="3">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
@@ -12199,10 +12199,10 @@
       </c>
       <c r="O4" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
@@ -12233,11 +12233,11 @@
         <v/>
       </c>
       <c r="O5" s="8" t="str">
-        <f t="shared" ref="O5:O11" ca="1" si="4">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G5,IF(I5="Yes","_CONSTANT","")))), "::source_field::", A5), "::target_field::", C5), "::position::", D5), "::length::", E5), "::format::", H5), "::constant::", J5), "::is_nullable::", IF(F5="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L5), "none", LOWER(L5))))</f>
-        <v>pxi_common.char_format(customer_code, 10, pxi_common.format_type_ltrim_zeros, pxi_common.is_not_nullable) || -- customer_code -&gt; CustomerNumber</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>pxi_common.char_format(customer_code, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- customer_code -&gt; CustomerNumber</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -12265,11 +12265,11 @@
         <v/>
       </c>
       <c r="O6" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>pxi_common.char_format(customer_name, 40, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- customer_name -&gt; Longname</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>pxi_common.char_format(customer_name, 40, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- customer_name -&gt; Longname</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="C7" s="1" t="s">
         <v>48</v>
       </c>
@@ -12297,11 +12297,11 @@
         <v/>
       </c>
       <c r="O7" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>pxi_common.char_format('Y', 1, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT 'Y' -&gt; PACSCustomer</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>pxi_common.char_format('Y', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT 'Y' -&gt; PACSCustomer</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
@@ -12332,11 +12332,11 @@
         <v/>
       </c>
       <c r="O8" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>pxi_common.char_format(payer_customer_code, 10, pxi_common.format_type_ltrim_zeros, pxi_common.is_nullable) || -- payer_customer_code -&gt; PayerCode</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>pxi_common.char_format(payer_customer_code, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_nullable) || -- payer_customer_code -&gt; PayerCode</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
@@ -12364,11 +12364,11 @@
         <v/>
       </c>
       <c r="O9" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>pxi_common.char_format(tax_exempt, 1, pxi_common.format_type_none, pxi_common.is_nullable) || -- tax_exempt -&gt; TaxExempt</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>pxi_common.char_format(tax_exempt, 1, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- tax_exempt -&gt; TaxExempt</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="C10" s="1" t="s">
         <v>50</v>
       </c>
@@ -12396,11 +12396,11 @@
         <v/>
       </c>
       <c r="O10" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>pxi_common.char_format('NZD', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT 'NZD' -&gt; DefaultCurrenty</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>pxi_common.char_format('NZD', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'NZD' -&gt; DefaultCurrenty</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="C11" s="1" t="s">
         <v>52</v>
       </c>
@@ -12428,11 +12428,11 @@
         <v/>
       </c>
       <c r="O11" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '149' -&gt; SalesOrg</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '149' -&gt; SalesOrg</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="H12" s="3"/>
     </row>
   </sheetData>
@@ -12442,20 +12442,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -12476,7 +12476,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -12515,7 +12515,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -12542,11 +12542,11 @@
         <v/>
       </c>
       <c r="O2" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
-        <v>pxi_common.char_format('301001', 6, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '301001' -&gt; ICRecordType</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
+        <v>pxi_common.char_format('301001', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '301001' -&gt; ICRecordType</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -12574,11 +12574,11 @@
         <v/>
       </c>
       <c r="O3" s="8" t="str">
-        <f t="shared" ref="O3:O8" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O3:O8" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -12607,10 +12607,10 @@
       </c>
       <c r="O4" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>159</v>
       </c>
@@ -12643,10 +12643,10 @@
       </c>
       <c r="O5" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(cust_code, 10, pxi_common.format_type_ltrim_zeros, pxi_common.is_not_nullable) || -- cust_code -&gt; CustomerNumber</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(cust_code, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- cust_code -&gt; CustomerNumber</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>160</v>
       </c>
@@ -12675,10 +12675,10 @@
       </c>
       <c r="O6" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(cust_name, 40, pxi_common.format_type_none, pxi_common.is_nullable) || -- cust_name -&gt; CustomerDescription</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(cust_name, 40, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- cust_name -&gt; CustomerDescription</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>161</v>
       </c>
@@ -12707,10 +12707,10 @@
       </c>
       <c r="O7" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(sales_org_code, 3, pxi_common.format_type_none, pxi_common.is_nullable) || -- sales_org_code -&gt; CustomerSalesOrg</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(sales_org_code, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- sales_org_code -&gt; CustomerSalesOrg</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>162</v>
       </c>
@@ -12742,19 +12742,19 @@
       </c>
       <c r="O8" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(parent_cust_code, 10, pxi_common.format_type_ltrim_zeros, pxi_common.is_nullable) || -- parent_cust_code -&gt; ParentCustomerNumber</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(parent_cust_code, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_nullable) || -- parent_cust_code -&gt; ParentCustomerNumber</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15">
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="H12" s="3"/>
     </row>
   </sheetData>
@@ -12764,20 +12764,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2:O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -12798,7 +12798,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -12837,7 +12837,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -12864,16 +12864,16 @@
         <v/>
       </c>
       <c r="O2" s="8" t="str">
-        <f t="shared" ref="O2:O8" ca="1" si="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
-        <v>pxi_common.char_format('347001', 6, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '347001' -&gt; ICRecordType</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
+        <v>pxi_common.char_format('347001', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '347001' -&gt; ICRecordType</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3" si="2">D2+E2</f>
+        <f t="shared" ref="D3" si="1">D2+E2</f>
         <v>6</v>
       </c>
       <c r="E3" s="1">
@@ -12896,11 +12896,11 @@
         <v/>
       </c>
       <c r="O3" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O3:O8" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -12928,11 +12928,11 @@
         <v/>
       </c>
       <c r="O4" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G4,IF(I4="Yes","_CONSTANT","")))), "::source_field::", A4), "::target_field::", C4), "::position::", D4), "::length::", E4), "::format::", H4), "::constant::", J4), "::is_nullable::", IF(F4="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L4), "none", LOWER(L4))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -12963,11 +12963,11 @@
         <v/>
       </c>
       <c r="O5" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format(company_code, 10, pxi_common.format_type_ltrim_zeros, pxi_common.is_not_nullable) || -- company_code -&gt; VendorNumber</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(company_code, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- company_code -&gt; VendorNumber</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
@@ -12995,11 +12995,11 @@
         <v/>
       </c>
       <c r="O6" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format(longname, 40, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- longname -&gt; Longname</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(longname, 40, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- longname -&gt; Longname</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="C7" s="1" t="s">
         <v>44</v>
       </c>
@@ -13027,11 +13027,11 @@
         <v/>
       </c>
       <c r="O7" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format('Y', 1, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT 'Y' -&gt; PACSVendor</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format('Y', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT 'Y' -&gt; PACSVendor</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="C8" s="1" t="s">
         <v>45</v>
       </c>
@@ -13059,14 +13059,14 @@
         <v/>
       </c>
       <c r="O8" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format('1', 1, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '1' -&gt; TaxExempt</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format('1', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '1' -&gt; TaxExempt</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="H12" s="3"/>
     </row>
   </sheetData>
@@ -13076,20 +13076,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -13110,7 +13110,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -13149,7 +13149,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="C2" s="1" t="s">
         <v>73</v>
       </c>
@@ -13176,11 +13176,11 @@
         <v/>
       </c>
       <c r="O2" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
-        <v>pxi_common.char_format('330002', 6, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '330002' -&gt; RecordType</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
+        <v>pxi_common.char_format('330002', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '330002' -&gt; RecordType</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -13208,16 +13208,16 @@
         <v/>
       </c>
       <c r="O3" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O3:O11" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" ref="D4:D10" si="2">D3+E3</f>
+        <f t="shared" ref="D4:D10" si="3">D3+E3</f>
         <v>9</v>
       </c>
       <c r="E4" s="1">
@@ -13240,16 +13240,16 @@
         <v/>
       </c>
       <c r="O4" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G4,IF(I4="Yes","_CONSTANT","")))), "::source_field::", A4), "::target_field::", C4), "::position::", D4), "::length::", E4), "::format::", H4), "::constant::", J4), "::is_nullable::", IF(F4="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L4), "none", LOWER(L4))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="C5" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="E5" s="1">
@@ -13271,15 +13271,15 @@
         <v>64</v>
       </c>
       <c r="M5" s="7" t="str">
-        <f t="shared" ref="M5:M10" si="3">IF(ISBLANK(H5),"",CONCATENATE(IF(LEN(H5)&lt;&gt;E5,"#",""),LEN(H5)))</f>
+        <f t="shared" ref="M5:M10" si="4">IF(ISBLANK(H5),"",CONCATENATE(IF(LEN(H5)&lt;&gt;E5,"#",""),LEN(H5)))</f>
         <v/>
       </c>
       <c r="O5" s="8" t="str">
-        <f t="shared" ref="O5:O10" ca="1" si="4">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G5,IF(I5="Yes","_CONSTANT","")))), "::source_field::", A5), "::target_field::", C5), "::position::", D5), "::length::", E5), "::format::", H5), "::constant::", J5), "::is_nullable::", IF(F5="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L5), "none", LOWER(L5))))</f>
-        <v>pxi_common.char_format('DIV_1', 10, pxi_common.format_type_ltrim_zeros, pxi_common.is_not_nullable) || -- CONSTANT 'DIV_1' -&gt; CustomerCode</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format('DIV_1', 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- CONSTANT 'DIV_1' -&gt; CustomerCode</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>123</v>
       </c>
@@ -13287,7 +13287,7 @@
         <v>116</v>
       </c>
       <c r="D6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="E6" s="1">
@@ -13303,15 +13303,15 @@
         <v>64</v>
       </c>
       <c r="M6" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O6" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>pxi_common.char_format(prodcode, 18, pxi_common.format_type_ltrim_zeros, pxi_common.is_not_nullable) || -- prodcode -&gt; MaterialCode</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(prodcode, 18, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- prodcode -&gt; MaterialCode</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
@@ -13319,7 +13319,7 @@
         <v>117</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="E7" s="1">
@@ -13336,15 +13336,15 @@
       </c>
       <c r="J7" s="10"/>
       <c r="M7" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="O7" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>pxi_common.date_format(startdate, 'yyyymmdd', pxi_common.is_not_nullable) || -- startdate -&gt; StartDate</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.date_format(startdate, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- startdate -&gt; StartDate</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>125</v>
       </c>
@@ -13352,7 +13352,7 @@
         <v>118</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="E8" s="1">
@@ -13368,15 +13368,15 @@
         <v>137</v>
       </c>
       <c r="M8" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="O8" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>pxi_common.date_format(enddate, 'yyyymmdd', pxi_common.is_nullable) || -- enddate -&gt; EndDate</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.date_format(enddate, 'yyyymmdd', pxi_common.fc_is_nullable) || -- enddate -&gt; EndDate</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -13384,7 +13384,7 @@
         <v>119</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="E9" s="1">
@@ -13400,20 +13400,20 @@
         <v>122</v>
       </c>
       <c r="M9" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="O9" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>pxi_common.numb_format(listprice, '999999990.00', pxi_common.is_nullable) || -- listprice -&gt; ListPrice</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.numb_format(listprice, '999999990.00', pxi_common.fc_is_nullable) || -- listprice -&gt; ListPrice</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>68</v>
       </c>
       <c r="E10" s="1">
@@ -13432,18 +13432,18 @@
         <v>51</v>
       </c>
       <c r="M10" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O10" s="8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>pxi_common.char_format('NZD', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT 'NZD' -&gt; Currency</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format('NZD', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'NZD' -&gt; Currency</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15">
       <c r="H12" s="3"/>
     </row>
   </sheetData>
@@ -13453,20 +13453,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -13487,7 +13487,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -13526,7 +13526,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -13553,11 +13553,11 @@
         <v/>
       </c>
       <c r="O2" s="8" t="str">
-        <f t="shared" ref="O2:O13" ca="1" si="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
-        <v>pxi_common.char_format('306001', 6, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '306001' -&gt; ICRecordType</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
+        <v>pxi_common.char_format('306001', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '306001' -&gt; ICRecordType</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -13565,7 +13565,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3:D13" si="2">D2+E2</f>
+        <f t="shared" ref="D3:D13" si="1">D2+E2</f>
         <v>6</v>
       </c>
       <c r="E3" s="1">
@@ -13588,11 +13588,11 @@
         <v/>
       </c>
       <c r="O3" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O3:O13" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -13600,7 +13600,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E4" s="1">
@@ -13620,11 +13620,11 @@
         <v/>
       </c>
       <c r="O4" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format(hdr_division_code, 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- hdr_division_code -&gt; PXDivisionCode</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(hdr_division_code, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- hdr_division_code -&gt; PXDivisionCode</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -13632,7 +13632,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E5" s="1">
@@ -13655,11 +13655,11 @@
         <v/>
       </c>
       <c r="O5" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format(sold_to_cust_code, 20, pxi_common.format_type_ltrim_zeros, pxi_common.is_not_nullable) || -- sold_to_cust_code -&gt; CustomerNumber</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(sold_to_cust_code, 20, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- sold_to_cust_code -&gt; CustomerNumber</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -13667,7 +13667,7 @@
         <v>32</v>
       </c>
       <c r="D6" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="E6" s="1">
@@ -13687,11 +13687,11 @@
         <v/>
       </c>
       <c r="O6" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format(billing_doc_num, 10, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- billing_doc_num -&gt; InvoiceNumber</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(billing_doc_num, 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- billing_doc_num -&gt; InvoiceNumber</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -13699,7 +13699,7 @@
         <v>33</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="E7" s="1">
@@ -13719,11 +13719,11 @@
         <v/>
       </c>
       <c r="O7" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format(billing_doc_line_num, 6, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- billing_doc_line_num -&gt; InvoiceLineNumber</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(billing_doc_line_num, 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- billing_doc_line_num -&gt; InvoiceLineNumber</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -13731,7 +13731,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="E8" s="1">
@@ -13754,11 +13754,11 @@
         <v/>
       </c>
       <c r="O8" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format(matl_entd, 18, pxi_common.format_type_ltrim_zeros, pxi_common.is_not_nullable) || -- matl_entd -&gt; Material</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(matl_entd, 18, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- matl_entd -&gt; Material</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -13766,7 +13766,7 @@
         <v>35</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="E9" s="1">
@@ -13789,11 +13789,11 @@
         <v>8</v>
       </c>
       <c r="O9" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.date_format(order_eff_date, 'yyyymmdd', pxi_common.is_not_nullable) || -- order_eff_date -&gt; OrderDate</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.date_format(order_eff_date, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- order_eff_date -&gt; OrderDate</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -13801,7 +13801,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>74</v>
       </c>
       <c r="E10" s="1">
@@ -13824,11 +13824,11 @@
         <v>8</v>
       </c>
       <c r="O10" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.date_format(billing_eff_date, 'yyyymmdd', pxi_common.is_not_nullable) || -- billing_eff_date -&gt; InvoiceDate</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.date_format(billing_eff_date, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- billing_eff_date -&gt; InvoiceDate</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -13836,7 +13836,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>82</v>
       </c>
       <c r="E11" s="1">
@@ -13859,11 +13859,11 @@
         <v>17</v>
       </c>
       <c r="O11" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.numb_format(billed_qty_base_uom, 'S9999999999990.00', pxi_common.is_not_nullable) || -- billed_qty_base_uom -&gt; QuantityInvoiced</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.numb_format(billed_qty_base_uom, 'S9999999999990.00', pxi_common.fc_is_not_nullable) || -- billed_qty_base_uom -&gt; QuantityInvoiced</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -13871,7 +13871,7 @@
         <v>38</v>
       </c>
       <c r="D12" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>99</v>
       </c>
       <c r="E12" s="1">
@@ -13894,11 +13894,11 @@
         <v>13</v>
       </c>
       <c r="O12" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.numb_format(billed_gsv, 'S999999990.00', pxi_common.is_not_nullable) || -- billed_gsv -&gt; GrossAmount</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.numb_format(billed_gsv, 'S999999990.00', pxi_common.fc_is_not_nullable) || -- billed_gsv -&gt; GrossAmount</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -13906,7 +13906,7 @@
         <v>39</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>112</v>
       </c>
       <c r="E13" s="1">
@@ -13926,23 +13926,23 @@
         <v/>
       </c>
       <c r="O13" s="8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>pxi_common.char_format(doc_currcy_code, 5, pxi_common.format_type_none, pxi_common.is_nullable) || -- doc_currcy_code -&gt; Currency</v>
-      </c>
-    </row>
-    <row r="22" spans="15:15" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>pxi_common.char_format(doc_currcy_code, 5, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- doc_currcy_code -&gt; Currency</v>
+      </c>
+    </row>
+    <row r="22" spans="15:15" ht="15">
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="15:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="15:15" ht="15">
       <c r="O23" s="9"/>
     </row>
-    <row r="24" spans="15:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="15:15" ht="15">
       <c r="O24" s="9"/>
     </row>
-    <row r="25" spans="15:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="15:15" ht="15">
       <c r="O25" s="9"/>
     </row>
-    <row r="26" spans="15:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="15:15" ht="15">
       <c r="O26" s="9"/>
     </row>
   </sheetData>
@@ -13952,20 +13952,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2:O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -13986,7 +13986,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -14025,7 +14025,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -14052,11 +14052,11 @@
         <v/>
       </c>
       <c r="O2" s="8" t="str">
-        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
-        <v>pxi_common.char_format('361001', 6, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '361001' -&gt; ICRecordType</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <f ca="1">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G2,IF(I2="Yes","_CONSTANT","")))), "::source_field::", A2), "::target_field::", C2), "::position::", D2), "::length::", E2), "::format::", H2), "::constant::", J2), "::is_nullable::", IF(F2="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L2), "none", LOWER(L2))))</f>
+        <v>pxi_common.char_format('361001', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '361001' -&gt; ICRecordType</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -14084,11 +14084,11 @@
         <v/>
       </c>
       <c r="O3" s="8" t="str">
-        <f t="shared" ref="O3:O18" ca="1" si="3">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.is_not_nullable", "pxi_common.is_nullable")), "::format_type::", CONCATENATE("pxi_common.format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O3:O18" ca="1" si="3">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -14117,10 +14117,10 @@
       </c>
       <c r="O4" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>193</v>
       </c>
@@ -14152,10 +14152,10 @@
       </c>
       <c r="O5" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format(bus_partner_ref, 10, pxi_common.format_type_ltrim_zeros, pxi_common.is_not_nullable) || -- bus_partner_ref -&gt; AccountCode</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(bus_partner_ref, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- bus_partner_ref -&gt; AccountCode</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>191</v>
       </c>
@@ -14184,10 +14184,10 @@
       </c>
       <c r="O6" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format(tax_cust_ref, 20, pxi_common.format_type_none, pxi_common.is_nullable) || -- tax_cust_ref -&gt; Reference</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(tax_cust_ref, 20, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- tax_cust_ref -&gt; Reference</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="C7" s="1" t="s">
         <v>142</v>
       </c>
@@ -14216,10 +14216,10 @@
       </c>
       <c r="O7" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format('A', 1, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT 'A' -&gt; ActionFlag</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format('A', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'A' -&gt; ActionFlag</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
@@ -14248,10 +14248,10 @@
       </c>
       <c r="O8" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format('1', 1, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '1' -&gt; Type</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format('1', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '1' -&gt; Type</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>152</v>
       </c>
@@ -14283,10 +14283,10 @@
       </c>
       <c r="O9" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.date_format(posting_date, 'yyyymmdd', pxi_common.is_not_nullable) || -- posting_date -&gt; Date</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.date_format(posting_date, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- posting_date -&gt; Date</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
         <v>153</v>
       </c>
@@ -14315,10 +14315,10 @@
       </c>
       <c r="O10" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format(claim_ref, 18, pxi_common.format_type_none, pxi_common.is_nullable) || -- claim_ref -&gt; Number</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(claim_ref, 18, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- claim_ref -&gt; Number</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="C11" s="1" t="s">
         <v>144</v>
       </c>
@@ -14348,10 +14348,10 @@
       </c>
       <c r="O11" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format('0', 18, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT '0' -&gt; ParentNumber</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format('0', 18, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '0' -&gt; ParentNumber</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
         <v>150</v>
       </c>
@@ -14381,10 +14381,10 @@
       </c>
       <c r="O12" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format(assignment_no, 65, pxi_common.format_type_none, pxi_common.is_nullable) || -- assignment_no -&gt; ExtReference</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(assignment_no, 65, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- assignment_no -&gt; ExtReference</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="C13" s="1" t="s">
         <v>146</v>
       </c>
@@ -14413,10 +14413,10 @@
       </c>
       <c r="O13" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format('', 80, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '' -&gt; InvoiceLink</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format('', 80, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '' -&gt; InvoiceLink</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
         <v>154</v>
       </c>
@@ -14445,10 +14445,10 @@
       </c>
       <c r="O14" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format(reason_code, 5, pxi_common.format_type_none, pxi_common.is_nullable) || -- reason_code -&gt; ReasonCode</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format(reason_code, 5, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- reason_code -&gt; ReasonCode</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
         <v>190</v>
       </c>
@@ -14480,10 +14480,10 @@
       </c>
       <c r="O15" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.numb_format(amount, '9999999990.00', pxi_common.is_not_nullable) || -- amount -&gt; Amount</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.numb_format(amount, '9999999990.00', pxi_common.fc_is_not_nullable) || -- amount -&gt; Amount</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
         <v>192</v>
       </c>
@@ -14515,10 +14515,10 @@
       </c>
       <c r="O16" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.numb_format(tax_amount, '9999999990.00', pxi_common.is_not_nullable) || -- tax_amount -&gt; TaxAmount</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.numb_format(tax_amount, '9999999990.00', pxi_common.fc_is_not_nullable) || -- tax_amount -&gt; TaxAmount</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15">
       <c r="C17" s="1" t="s">
         <v>149</v>
       </c>
@@ -14547,10 +14547,10 @@
       </c>
       <c r="O17" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format('', 256, pxi_common.format_type_none, pxi_common.is_nullable) || -- CONSTANT '' -&gt; Note</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.2">
+        <v>pxi_common.char_format('', 256, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '' -&gt; Note</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15">
       <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
@@ -14579,7 +14579,7 @@
       </c>
       <c r="O18" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format('NZD', 3, pxi_common.format_type_none, pxi_common.is_not_nullable) || -- CONSTANT 'NZD' -&gt; Currency</v>
+        <v>pxi_common.char_format('NZD', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'NZD' -&gt; Currency</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated so that the product status is generated from the query in PXIPMX01_EXTRACT
</commit_message>
<xml_diff>
--- a/SOURCE/PXI/DOC/Promax Interface Format 20130802_3.xlsx
+++ b/SOURCE/PXI/DOC/Promax Interface Format 20130802_3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20730" windowHeight="4245" tabRatio="635" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20730" windowHeight="4245" tabRatio="635" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Interface Master" sheetId="14" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="446">
   <si>
     <t>No</t>
   </si>
@@ -1380,6 +1380,9 @@
   </si>
   <si>
     <t>Order Type Code</t>
+  </si>
+  <si>
+    <t>product_status</t>
   </si>
 </sst>
 </file>
@@ -3022,7 +3025,7 @@
   </sheetPr>
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
@@ -10893,11 +10896,11 @@
   </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
+      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -11125,6 +11128,9 @@
       </c>
     </row>
     <row r="7" spans="1:15">
+      <c r="A7" s="1" t="s">
+        <v>445</v>
+      </c>
       <c r="C7" s="1" t="s">
         <v>75</v>
       </c>
@@ -11142,18 +11148,16 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>106</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J7" s="10"/>
       <c r="M7" s="7" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="O7" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format('1', 2, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '1' -&gt; Status</v>
+        <v>pxi_common.char_format(product_status, 2, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- product_status -&gt; Status</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -13208,7 +13212,7 @@
         <v/>
       </c>
       <c r="O3" s="8" t="str">
-        <f t="shared" ref="O3:O11" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
+        <f t="shared" ref="O3:O10" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed ord_doc_line_num to 10 from 6
</commit_message>
<xml_diff>
--- a/SOURCE/PXI/DOC/Promax Interface Format 20130802_3.xlsx
+++ b/SOURCE/PXI/DOC/Promax Interface Format 20130802_3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20730" windowHeight="4245" tabRatio="635" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20730" windowHeight="4245" tabRatio="635" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Interface Master" sheetId="14" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="14">'FFLU PMXPXI03 - 359PROM'!$A$1:$J$40</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="10">'PXIATL02 - CISATL14'!$A$1:$L$19</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1388,8 +1388,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1565,6 +1565,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1599,6 +1600,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1774,7 +1776,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1782,7 +1784,7 @@
       <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1800,7 +1802,7 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1">
+    <row r="1" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>194</v>
       </c>
@@ -1829,7 +1831,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1858,7 +1860,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1887,7 +1889,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1916,7 +1918,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1945,7 +1947,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1974,7 +1976,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2003,7 +2005,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2026,7 +2028,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2055,7 +2057,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2081,7 +2083,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2104,7 +2106,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2130,7 +2132,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2159,7 +2161,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2185,7 +2187,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2211,7 +2213,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2252,7 +2254,7 @@
         <v>site_app.pmxpxi03_loader</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2281,7 +2283,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2322,7 +2324,7 @@
         <v>site_app.pmxpxi01_loader</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2351,7 +2353,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2392,7 +2394,7 @@
         <v>site_app.pmxpxi02_loader</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2421,7 +2423,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2450,7 +2452,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2479,7 +2481,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2516,7 +2518,7 @@
         <v>Promax NZ &gt; DFN : Demand : 337 : 337EST</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2542,7 +2544,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2562,7 +2564,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2582,17 +2584,17 @@
         <v>198</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>237</v>
       </c>
@@ -2604,7 +2606,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -2617,7 +2619,7 @@
       <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -2638,7 +2640,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -2677,7 +2679,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>73</v>
       </c>
@@ -2708,7 +2710,7 @@
         <v>pxi_common.char_format('336002', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '336002' -&gt; RecordType</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -2740,7 +2742,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -2772,7 +2774,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>169</v>
       </c>
@@ -2804,7 +2806,7 @@
         <v>pxi_common.char_format(invoicenumber, 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- invoicenumber -&gt; InvoiceNumber</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>170</v>
       </c>
@@ -2836,7 +2838,7 @@
         <v>pxi_common.char_format(invoicelinenumber, 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- invoicelinenumber -&gt; InvoiceLineNumber</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>171</v>
       </c>
@@ -2872,7 +2874,7 @@
         <v>pxi_common.char_format(customerhierarchy, 8, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- customerhierarchy -&gt; CustomerHierarchy</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>172</v>
       </c>
@@ -2908,7 +2910,7 @@
         <v>pxi_common.char_format(material, 18, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- material -&gt; Material</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>173</v>
       </c>
@@ -2943,7 +2945,7 @@
         <v>pxi_common.date_format(invoicedate, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- invoicedate -&gt; InvoiceDate</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>174</v>
       </c>
@@ -2978,7 +2980,7 @@
         <v>pxi_common.numb_format(discountgiven, '9999990.00', pxi_common.fc_is_not_nullable) || -- discountgiven -&gt; DiscountGiven</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>175</v>
       </c>
@@ -3018,7 +3020,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
@@ -3029,7 +3031,7 @@
       <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -3050,7 +3052,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -3089,7 +3091,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>406</v>
       </c>
@@ -3120,7 +3122,7 @@
         <v>pxi_common.char_format('A', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'A' -&gt; UsageConditionCode</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>407</v>
       </c>
@@ -3153,7 +3155,7 @@
         <v>pxi_common.char_format(cndtn_table_ref, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- cndtn_table_ref -&gt; CondTable</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>409</v>
       </c>
@@ -3185,7 +3187,7 @@
         <v>pxi_common.char_format('V', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'V' -&gt; Application</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>411</v>
       </c>
@@ -3217,7 +3219,7 @@
         <v>pxi_common.char_format(VAKEY, 50, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- VAKEY -&gt; VAKEY</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>412</v>
       </c>
@@ -3249,7 +3251,7 @@
         <v>pxi_common.char_format(px_company_code, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- px_company_code -&gt; CompanyCode</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>414</v>
       </c>
@@ -3282,7 +3284,7 @@
         <v>pxi_common.char_format(cust_div_code, 2, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- cust_div_code -&gt; Division</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>416</v>
       </c>
@@ -3315,7 +3317,7 @@
         <v>pxi_common.char_format(cust_hier, 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- cust_hier -&gt; Customer</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>172</v>
       </c>
@@ -3348,7 +3350,7 @@
         <v>pxi_common.char_format(material, 18, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- material -&gt; Material</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>418</v>
       </c>
@@ -3383,7 +3385,7 @@
         <v>pxi_common.date_format(buy_start_date, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- buy_start_date -&gt; ValidFrom</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>420</v>
       </c>
@@ -3418,7 +3420,7 @@
         <v>pxi_common.date_format(buy_stop_date, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- buy_stop_date -&gt; ValidTo</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>422</v>
       </c>
@@ -3451,7 +3453,7 @@
         <v>pxi_common.char_format(pricing_cndtn_code, 4, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- pricing_cndtn_code -&gt; Condition</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>424</v>
       </c>
@@ -3486,7 +3488,7 @@
         <v>pxi_common.char_format(condition_type_code, 1, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- condition_type_code -&gt; ConditionType</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>425</v>
       </c>
@@ -3521,7 +3523,7 @@
         <v>pxi_common.numb_format(rate, 's9999990.00', pxi_common.fc_is_not_nullable) || -- rate -&gt; Rate</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>427</v>
       </c>
@@ -3554,7 +3556,7 @@
         <v>pxi_common.char_format(rate_unit, 5, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- rate_unit -&gt; RateUnit</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
         <v>79</v>
       </c>
@@ -3587,7 +3589,7 @@
         <v>pxi_common.char_format('EA', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'EA' -&gt; UOM</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>430</v>
       </c>
@@ -3622,7 +3624,7 @@
         <v>pxi_common.char_format(sales_deal, 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- sales_deal -&gt; PromoNum</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>432</v>
       </c>
@@ -3654,7 +3656,7 @@
         <v>pxi_common.char_format(rate_multiplier, 5, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- rate_multiplier -&gt; PriceUnit</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>434</v>
       </c>
@@ -3693,7 +3695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -3706,7 +3708,7 @@
       <selection pane="bottomRight" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="8" bestFit="1" customWidth="1"/>
@@ -3725,7 +3727,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" ht="11.25">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>275</v>
       </c>
@@ -3769,7 +3771,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="11.25">
+    <row r="2" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>283</v>
       </c>
@@ -3838,7 +3840,7 @@
         <v>rec_type varchar2(3 char),</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="11.25">
+    <row r="3" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>285</v>
       </c>
@@ -3908,7 +3910,7 @@
         <v>idoc_type varchar2(30 char),</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="11.25">
+    <row r="4" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>287</v>
       </c>
@@ -3981,7 +3983,7 @@
         <v>idoc_no number(16,0),</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="11.25">
+    <row r="5" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>290</v>
       </c>
@@ -4054,7 +4056,7 @@
         <v>idoc_date date,</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="11.25">
+    <row r="6" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4069,7 +4071,7 @@
       </c>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:14" ht="11.25">
+    <row r="7" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>283</v>
       </c>
@@ -4138,7 +4140,7 @@
         <v>rec_type varchar2(3 char),</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="11.25">
+    <row r="8" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>292</v>
       </c>
@@ -4187,7 +4189,7 @@
         <v>company_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="11.25">
+    <row r="9" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>293</v>
       </c>
@@ -4236,7 +4238,7 @@
         <v>div_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="11.25">
+    <row r="10" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>294</v>
       </c>
@@ -4285,7 +4287,7 @@
         <v>cust_code varchar2(10 char),</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="11.25">
+    <row r="11" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>296</v>
       </c>
@@ -4337,7 +4339,7 @@
         <v>claim_amount number(15,4),</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="11.25">
+    <row r="12" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>299</v>
       </c>
@@ -4386,7 +4388,7 @@
         <v>claim_ref varchar2(12 char),</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="11.25">
+    <row r="13" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>301</v>
       </c>
@@ -4435,7 +4437,7 @@
         <v>assignment_no varchar2(18 char),</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="11.25">
+    <row r="14" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>303</v>
       </c>
@@ -4487,7 +4489,7 @@
         <v>tax_base number(15,4),</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="11.25">
+    <row r="15" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>304</v>
       </c>
@@ -4539,7 +4541,7 @@
         <v>posting_date date,</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="11.25">
+    <row r="16" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>305</v>
       </c>
@@ -4591,7 +4593,7 @@
         <v>fiscal_period number(2,0),</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="11.25">
+    <row r="17" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>308</v>
       </c>
@@ -4640,7 +4642,7 @@
         <v>reason_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="11.25">
+    <row r="18" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>309</v>
       </c>
@@ -4690,7 +4692,7 @@
         <v>accounting_doc_no varchar2(10 char),</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="11.25">
+    <row r="19" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>310</v>
       </c>
@@ -4742,7 +4744,7 @@
         <v>fiscal_year number(4,0),</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="11.25">
+    <row r="20" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>313</v>
       </c>
@@ -4792,7 +4794,7 @@
         <v>line_item_no varchar2(3),</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="11.25">
+    <row r="21" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>315</v>
       </c>
@@ -4841,7 +4843,7 @@
         <v>bus_partner_ref varchar2(12 char),</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="11.25">
+    <row r="22" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>316</v>
       </c>
@@ -4890,43 +4892,43 @@
         <v>tax_code varchar2(2 char),</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="11.25">
+    <row r="23" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K23" s="8"/>
     </row>
-    <row r="24" spans="1:14" ht="11.25">
+    <row r="24" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="1:14" ht="11.25">
+    <row r="25" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K25" s="8"/>
     </row>
-    <row r="26" spans="1:14" ht="11.25">
+    <row r="26" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K26" s="8"/>
     </row>
-    <row r="27" spans="1:14" ht="11.25">
+    <row r="27" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K27" s="8"/>
     </row>
-    <row r="28" spans="1:14" ht="11.25">
+    <row r="28" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K28" s="8"/>
     </row>
-    <row r="29" spans="1:14" ht="11.25">
+    <row r="29" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K29" s="8"/>
     </row>
-    <row r="30" spans="1:14" ht="11.25">
+    <row r="30" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K30" s="8"/>
     </row>
-    <row r="31" spans="1:14" ht="11.25">
+    <row r="31" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K31" s="8"/>
     </row>
-    <row r="32" spans="1:14" ht="11.25">
+    <row r="32" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K32" s="8"/>
     </row>
-    <row r="33" spans="11:11" s="1" customFormat="1" ht="11.25">
+    <row r="33" spans="11:11" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K33" s="8"/>
     </row>
-    <row r="34" spans="11:11" s="1" customFormat="1" ht="11.25">
+    <row r="34" spans="11:11" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K34" s="8"/>
     </row>
-    <row r="35" spans="11:11" s="1" customFormat="1" ht="11.25">
+    <row r="35" spans="11:11" s="1" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K35" s="8"/>
     </row>
   </sheetData>
@@ -4935,7 +4937,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -4948,7 +4950,7 @@
       <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="8" bestFit="1" customWidth="1"/>
@@ -4967,7 +4969,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" ht="11.25">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>275</v>
       </c>
@@ -5011,7 +5013,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="11.25">
+    <row r="2" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>318</v>
       </c>
@@ -5080,7 +5082,7 @@
         <v>ic_record_type varchar2(6 char),</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="11.25">
+    <row r="3" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>320</v>
       </c>
@@ -5150,7 +5152,7 @@
         <v>px_company_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="11.25">
+    <row r="4" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>321</v>
       </c>
@@ -5199,7 +5201,7 @@
         <v>px_division_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="11.25">
+    <row r="5" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>283</v>
       </c>
@@ -5248,7 +5250,7 @@
         <v>rec_type varchar2(1 char),</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="11.25">
+    <row r="6" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>323</v>
       </c>
@@ -5300,7 +5302,7 @@
         <v>document_date date,</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="11.25">
+    <row r="7" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>304</v>
       </c>
@@ -5352,7 +5354,7 @@
         <v>posting_date date,</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="11.25">
+    <row r="8" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>324</v>
       </c>
@@ -5401,7 +5403,7 @@
         <v>document_type varchar2(2 char),</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="11.25">
+    <row r="9" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -5450,7 +5452,7 @@
         <v>currency varchar2(3 char),</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="11.25">
+    <row r="10" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>141</v>
       </c>
@@ -5499,7 +5501,7 @@
         <v>reference varchar2(16 char),</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="11.25">
+    <row r="11" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>326</v>
       </c>
@@ -5548,7 +5550,7 @@
         <v>document_header_text varchar2(25 char),</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="11.25">
+    <row r="12" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>328</v>
       </c>
@@ -5597,7 +5599,7 @@
         <v>posting_key varchar2(4 char),</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="11.25">
+    <row r="13" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>179</v>
       </c>
@@ -5646,7 +5648,7 @@
         <v>account varchar2(17 char),</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="11.25">
+    <row r="14" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>331</v>
       </c>
@@ -5695,7 +5697,7 @@
         <v>pa_assignment_flag varchar2(1 char),</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="11.25">
+    <row r="15" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>148</v>
       </c>
@@ -5747,7 +5749,7 @@
         <v>amount number(13,2),</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="11.25">
+    <row r="16" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>332</v>
       </c>
@@ -5796,7 +5798,7 @@
         <v>payment_method varchar2(1 char),</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="11.25">
+    <row r="17" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>181</v>
       </c>
@@ -5845,7 +5847,7 @@
         <v>allocation varchar2(18 char),</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="11.25">
+    <row r="18" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>182</v>
       </c>
@@ -5894,7 +5896,7 @@
         <v>text varchar2(30 char),</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="11.25">
+    <row r="19" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>333</v>
       </c>
@@ -5943,7 +5945,7 @@
         <v>profit_centre varchar2(10 char),</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="11.25">
+    <row r="20" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>334</v>
       </c>
@@ -5992,7 +5994,7 @@
         <v>cost_centre varchar2(10 char),</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="11.25">
+    <row r="21" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>335</v>
       </c>
@@ -6041,7 +6043,7 @@
         <v>sales_organisation varchar2(4 char),</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="11.25">
+    <row r="22" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>336</v>
       </c>
@@ -6090,7 +6092,7 @@
         <v>sales_office varchar2(5 char),</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="11.25">
+    <row r="23" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>338</v>
       </c>
@@ -6139,7 +6141,7 @@
         <v>product_number varchar2(18 char),</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="11.25">
+    <row r="24" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>339</v>
       </c>
@@ -6188,7 +6190,7 @@
         <v>pa_code varchar2(5 char),</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="11.25">
+    <row r="25" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>340</v>
       </c>
@@ -6237,7 +6239,7 @@
         <v>glt_row_id varchar2(10 char),</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="11.25">
+    <row r="26" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>341</v>
       </c>
@@ -6286,7 +6288,7 @@
         <v>user_1 varchar2(10 char),</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="11.25">
+    <row r="27" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>342</v>
       </c>
@@ -6335,7 +6337,7 @@
         <v>user_2 varchar2(10 char),</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="11.25">
+    <row r="28" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>343</v>
       </c>
@@ -6387,7 +6389,7 @@
         <v>buy_start_date date,</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="11.25">
+    <row r="29" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>344</v>
       </c>
@@ -6439,7 +6441,7 @@
         <v>buy_stop_date date,</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="11.25">
+    <row r="30" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>345</v>
       </c>
@@ -6491,7 +6493,7 @@
         <v>start_date date,</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="11.25">
+    <row r="31" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>346</v>
       </c>
@@ -6543,7 +6545,7 @@
         <v>stop_date date,</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="11.25">
+    <row r="32" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>183</v>
       </c>
@@ -6592,7 +6594,7 @@
         <v>quantity varchar2(15 char),</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="11.25">
+    <row r="33" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>348</v>
       </c>
@@ -6641,7 +6643,7 @@
         <v>additional_info varchar2(10 char),</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="11.25">
+    <row r="34" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>349</v>
       </c>
@@ -6690,7 +6692,7 @@
         <v>promotion_is_closed varchar2(1 char),</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="11.25">
+    <row r="35" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="K35" s="8"/>
     </row>
   </sheetData>
@@ -6699,7 +6701,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
@@ -6712,7 +6714,7 @@
       <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" style="16" bestFit="1" customWidth="1"/>
@@ -6731,7 +6733,7 @@
     <col min="15" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="16" customFormat="1" ht="11.25">
+    <row r="1" spans="1:14" s="16" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>275</v>
       </c>
@@ -6775,7 +6777,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="11.25">
+    <row r="2" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>318</v>
       </c>
@@ -6844,7 +6846,7 @@
         <v>ic_record_type varchar2(6 char),</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="11.25">
+    <row r="3" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>320</v>
       </c>
@@ -6907,7 +6909,7 @@
         <v>px_company_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="11.25">
+    <row r="4" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>321</v>
       </c>
@@ -6956,7 +6958,7 @@
         <v>px_division_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="11.25">
+    <row r="5" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>8</v>
       </c>
@@ -7005,7 +7007,7 @@
         <v>type varchar2(1 char),</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="11.25">
+    <row r="6" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>323</v>
       </c>
@@ -7057,7 +7059,7 @@
         <v>document_date date,</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="11.25">
+    <row r="7" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>304</v>
       </c>
@@ -7109,7 +7111,7 @@
         <v>posting_date date,</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="11.25">
+    <row r="8" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>350</v>
       </c>
@@ -7161,7 +7163,7 @@
         <v>claim_date date,</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="11.25">
+    <row r="9" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>141</v>
       </c>
@@ -7210,7 +7212,7 @@
         <v>reference varchar2(10 char),</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="11.25">
+    <row r="10" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>326</v>
       </c>
@@ -7259,7 +7261,7 @@
         <v>document_header_text varchar2(25 char),</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="11.25">
+    <row r="11" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>351</v>
       </c>
@@ -7308,7 +7310,7 @@
         <v>expenditure_type varchar2(5 char),</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="11.25">
+    <row r="12" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>328</v>
       </c>
@@ -7357,7 +7359,7 @@
         <v>posting_key varchar2(7 char),</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="11.25">
+    <row r="13" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>353</v>
       </c>
@@ -7406,7 +7408,7 @@
         <v>account_code varchar2(10 char),</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="11.25">
+    <row r="14" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>148</v>
       </c>
@@ -7458,7 +7460,7 @@
         <v>amount number(14,2),</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="11.25">
+    <row r="15" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>354</v>
       </c>
@@ -7510,7 +7512,7 @@
         <v>spend_amount number(14,2),</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="11.25">
+    <row r="16" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>355</v>
       </c>
@@ -7562,7 +7564,7 @@
         <v>tax_amount number(14,2),</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="11.25">
+    <row r="17" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
         <v>332</v>
       </c>
@@ -7611,7 +7613,7 @@
         <v>payment_method varchar2(1 char),</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="11.25">
+    <row r="18" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>181</v>
       </c>
@@ -7660,7 +7662,7 @@
         <v>allocation varchar2(12 char),</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="11.25">
+    <row r="19" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
         <v>356</v>
       </c>
@@ -7709,7 +7711,7 @@
         <v>pc_reference varchar2(18 char),</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="11.25">
+    <row r="20" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
         <v>357</v>
       </c>
@@ -7758,7 +7760,7 @@
         <v>px_reference varchar2(60 char),</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="11.25">
+    <row r="21" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
         <v>359</v>
       </c>
@@ -7807,7 +7809,7 @@
         <v>ext_reference varchar2(65 char),</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="11.25">
+    <row r="22" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
         <v>338</v>
       </c>
@@ -7856,7 +7858,7 @@
         <v>product_number varchar2(18 char),</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="11.25">
+    <row r="23" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
         <v>361</v>
       </c>
@@ -7905,7 +7907,7 @@
         <v>transaction_code varchar2(40 char),</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="11.25">
+    <row r="24" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
         <v>363</v>
       </c>
@@ -7954,7 +7956,7 @@
         <v>deduction_ac_code varchar2(20 char),</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="11.25">
+    <row r="25" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
         <v>365</v>
       </c>
@@ -8003,7 +8005,7 @@
         <v>payee_code varchar2(10 char),</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="11.25">
+    <row r="26" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
         <v>366</v>
       </c>
@@ -8052,7 +8054,7 @@
         <v>debit_code varchar2(20 char),</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="11.25">
+    <row r="27" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
         <v>367</v>
       </c>
@@ -8101,7 +8103,7 @@
         <v>credit_code varchar2(20 char),</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="11.25">
+    <row r="28" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
         <v>368</v>
       </c>
@@ -8150,7 +8152,7 @@
         <v>customer_is_a_vendor varchar2(1 char),</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="11.25">
+    <row r="29" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
         <v>39</v>
       </c>
@@ -8199,7 +8201,7 @@
         <v>currency varchar2(3 char),</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="11.25">
+    <row r="30" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
         <v>369</v>
       </c>
@@ -8248,7 +8250,7 @@
         <v>promo_claim_detail_row_id varchar2(10 char),</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="11.25">
+    <row r="31" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
         <v>370</v>
       </c>
@@ -8297,7 +8299,7 @@
         <v>promo_claim_group_row_id varchar2(10 char),</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="11.25">
+    <row r="32" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
         <v>371</v>
       </c>
@@ -8346,7 +8348,7 @@
         <v>promo_claim_group_pub_id varchar2(30 char),</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="11.25">
+    <row r="33" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
         <v>308</v>
       </c>
@@ -8395,7 +8397,7 @@
         <v>reason_code varchar2(5 char),</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="11.25">
+    <row r="34" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
         <v>372</v>
       </c>
@@ -8444,7 +8446,7 @@
         <v>pc_message varchar2(65 char),</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="11.25">
+    <row r="35" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>373</v>
       </c>
@@ -8493,7 +8495,7 @@
         <v>pc_comment varchar2(200 char),</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="11.25">
+    <row r="36" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
         <v>375</v>
       </c>
@@ -8542,7 +8544,7 @@
         <v>text_1 varchar2(40 char),</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="11.25">
+    <row r="37" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
         <v>376</v>
       </c>
@@ -8591,7 +8593,7 @@
         <v>text_2 varchar2(40 char),</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="11.25">
+    <row r="38" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
         <v>343</v>
       </c>
@@ -8643,7 +8645,7 @@
         <v>buy_start_date date,</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="11.25">
+    <row r="39" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
         <v>344</v>
       </c>
@@ -8695,7 +8697,7 @@
         <v>buy_stop_date date,</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="11.25">
+    <row r="40" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
         <v>377</v>
       </c>
@@ -8750,7 +8752,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
@@ -8764,7 +8766,7 @@
       <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="8" bestFit="1" customWidth="1"/>
@@ -8783,7 +8785,7 @@
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="8" customFormat="1" ht="11.25">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>275</v>
       </c>
@@ -8827,7 +8829,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="11.25">
+    <row r="2" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>318</v>
       </c>
@@ -8896,7 +8898,7 @@
         <v>ic_record_type varchar2(6 char),</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="11.25">
+    <row r="3" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>320</v>
       </c>
@@ -8959,7 +8961,7 @@
         <v>px_company_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="11.25">
+    <row r="4" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>321</v>
       </c>
@@ -9008,7 +9010,7 @@
         <v>px_division_code varchar2(3 char),</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="11.25">
+    <row r="5" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>210</v>
       </c>
@@ -9057,7 +9059,7 @@
         <v>customer_hierarchy varchar2(10 char),</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="11.25">
+    <row r="6" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>378</v>
       </c>
@@ -9106,7 +9108,7 @@
         <v>sales_deal varchar2(10 char),</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="11.25">
+    <row r="7" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -9155,7 +9157,7 @@
         <v>material varchar2(18 char),</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="11.25">
+    <row r="8" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>343</v>
       </c>
@@ -9207,7 +9209,7 @@
         <v>buy_start_date date,</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="11.25">
+    <row r="9" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>344</v>
       </c>
@@ -9259,7 +9261,7 @@
         <v>buy_stop_date date,</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="11.25">
+    <row r="10" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>361</v>
       </c>
@@ -9308,7 +9310,7 @@
         <v>transaction_code varchar2(4 char),</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="11.25">
+    <row r="11" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>109</v>
       </c>
@@ -9357,7 +9359,7 @@
         <v>description varchar2(40 char),</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="11.25">
+    <row r="12" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>379</v>
       </c>
@@ -9406,7 +9408,7 @@
         <v>sales_org varchar2(4 char),</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="11.25">
+    <row r="13" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>176</v>
       </c>
@@ -9458,7 +9460,7 @@
         <v>rate number(12,2),</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="11.25">
+    <row r="14" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>341</v>
       </c>
@@ -9507,7 +9509,7 @@
         <v>user_1 varchar2(10 char),</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="11.25">
+    <row r="15" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>342</v>
       </c>
@@ -9556,7 +9558,7 @@
         <v>user_2 varchar2(10 char),</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="11.25">
+    <row r="16" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>380</v>
       </c>
@@ -9605,7 +9607,7 @@
         <v>action_code varchar2(1 char),</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="11.25">
+    <row r="17" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>381</v>
       </c>
@@ -9654,7 +9656,7 @@
         <v>bonus_stock_description varchar2(100 char),</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="11.25">
+    <row r="18" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>383</v>
       </c>
@@ -9706,7 +9708,7 @@
         <v>bonus_stock_hurdle number(9,2),</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="11.25">
+    <row r="19" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>384</v>
       </c>
@@ -9758,7 +9760,7 @@
         <v>bonus_stock_receive number(9,2),</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="11.25">
+    <row r="20" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>385</v>
       </c>
@@ -9807,7 +9809,7 @@
         <v>bonus_stock_sku_code varchar2(18 char),</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="11.25">
+    <row r="21" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>386</v>
       </c>
@@ -9856,7 +9858,7 @@
         <v>rate_unit varchar2(5 char),</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="11.25">
+    <row r="22" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>387</v>
       </c>
@@ -9905,7 +9907,7 @@
         <v>condition_pricing_unit varchar2(5 char),</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="11.25">
+    <row r="23" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>388</v>
       </c>
@@ -9954,7 +9956,7 @@
         <v>condition_uom varchar2(3 char),</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="11.25">
+    <row r="24" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>389</v>
       </c>
@@ -10003,7 +10005,7 @@
         <v>sap_promo_number varchar2(10 char),</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="11.25">
+    <row r="25" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>39</v>
       </c>
@@ -10052,7 +10054,7 @@
         <v>currency varchar2(3 char),</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="11.25">
+    <row r="26" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>390</v>
       </c>
@@ -10101,7 +10103,7 @@
         <v>uom_str_unit varchar2(3 char),</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="11.25">
+    <row r="27" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>391</v>
       </c>
@@ -10150,7 +10152,7 @@
         <v>uom_str_saleable varchar2(3 char),</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="11.25">
+    <row r="28" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>392</v>
       </c>
@@ -10199,7 +10201,7 @@
         <v>promo_price_saleable varchar2(10 char),</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="11.25">
+    <row r="29" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>393</v>
       </c>
@@ -10248,7 +10250,7 @@
         <v>promo_price_unit varchar2(10 char),</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="11.25">
+    <row r="30" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>394</v>
       </c>
@@ -10297,7 +10299,7 @@
         <v>transaction_amount varchar2(10 char),</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="11.25">
+    <row r="31" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>395</v>
       </c>
@@ -10346,14 +10348,14 @@
         <v>payer_code varchar2(20 char),</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="11.25">
+    <row r="32" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="I32" s="7" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="K32" s="8"/>
     </row>
-    <row r="33" spans="1:14" ht="11.25">
+    <row r="33" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>436</v>
       </c>
@@ -10399,7 +10401,7 @@
         <v>condition_flag varchar2(1 char),</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="11.25">
+    <row r="34" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>437</v>
       </c>
@@ -10445,7 +10447,7 @@
         <v>business_segment varchar2(2 char),</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="11.25">
+    <row r="35" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>438</v>
       </c>
@@ -10491,7 +10493,7 @@
         <v>rate_multiplier number(4),</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="11.25">
+    <row r="36" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>440</v>
       </c>
@@ -10537,7 +10539,7 @@
         <v>condition_type_code varchar2(1 char),</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="11.25">
+    <row r="37" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>441</v>
       </c>
@@ -10583,7 +10585,7 @@
         <v>pricing_condition_code varchar2(4 char),</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="11.25">
+    <row r="38" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>442</v>
       </c>
@@ -10629,7 +10631,7 @@
         <v>condition_table_ref varchar2(5 char),</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="11.25">
+    <row r="39" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>443</v>
       </c>
@@ -10675,7 +10677,7 @@
         <v>cust_div_code varchar2(2 char),</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="11.25">
+    <row r="40" spans="1:14" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>444</v>
       </c>
@@ -10728,7 +10730,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -10739,14 +10741,14 @@
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="130.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="6" customFormat="1">
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -10754,15 +10756,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="13" customFormat="1">
+    <row r="2" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
     </row>
-    <row r="3" spans="1:2" s="6" customFormat="1">
+    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
@@ -10770,7 +10772,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>23</v>
       </c>
@@ -10778,7 +10780,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
@@ -10786,7 +10788,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -10794,7 +10796,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>72</v>
       </c>
@@ -10802,32 +10804,32 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="8" customFormat="1">
+    <row r="15" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>259</v>
       </c>
@@ -10835,7 +10837,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>261</v>
       </c>
@@ -10843,7 +10845,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>263</v>
       </c>
@@ -10851,7 +10853,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>265</v>
       </c>
@@ -10859,7 +10861,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>267</v>
       </c>
@@ -10867,7 +10869,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>269</v>
       </c>
@@ -10875,7 +10877,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>271</v>
       </c>
@@ -10890,20 +10892,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -10924,7 +10926,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -10963,7 +10965,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>73</v>
       </c>
@@ -10994,7 +10996,7 @@
         <v>pxi_common.char_format('302001', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '302001' -&gt; RecordType</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -11027,7 +11029,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -11060,7 +11062,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>92</v>
       </c>
@@ -11095,7 +11097,7 @@
         <v>pxi_common.char_format(zrep_matl_code, 18, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- zrep_matl_code -&gt; ProductItemNumber</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>93</v>
       </c>
@@ -11127,7 +11129,7 @@
         <v>pxi_common.char_format(zrep_matl_desc, 40, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- zrep_matl_desc -&gt; Description</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>445</v>
       </c>
@@ -11160,7 +11162,7 @@
         <v>pxi_common.char_format(product_status, 2, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- product_status -&gt; Status</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>92</v>
       </c>
@@ -11195,7 +11197,7 @@
         <v>pxi_common.char_format(zrep_matl_code, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_nullable) || -- zrep_matl_code -&gt; ShortName</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>94</v>
       </c>
@@ -11227,7 +11229,7 @@
         <v>pxi_common.char_format(rsu_ean, 18, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- rsu_ean -&gt; APN</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>95</v>
       </c>
@@ -11259,7 +11261,7 @@
         <v>pxi_common.char_format(tdu_ean, 18, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- tdu_ean -&gt; TUN</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>110</v>
       </c>
@@ -11291,7 +11293,7 @@
         <v>pxi_common.char_format(rsu_uom, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- rsu_uom -&gt; UOM</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>96</v>
       </c>
@@ -11324,7 +11326,7 @@
         <v>pxi_common.char_format(tdu_uom, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- tdu_uom -&gt; SellableUOM</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>104</v>
       </c>
@@ -11359,7 +11361,7 @@
         <v>pxi_common.numb_format(rsus_per_tdu, '99999999999990', pxi_common.fc_is_nullable) || -- rsus_per_tdu -&gt; UnitsPerCase</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>104</v>
       </c>
@@ -11394,7 +11396,7 @@
         <v>pxi_common.numb_format(rsus_per_tdu, '99999999999990', pxi_common.fc_is_nullable) || -- rsus_per_tdu -&gt; BaseUnitsPerSellable</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
@@ -11426,7 +11428,7 @@
         <v>pxi_common.char_format('0', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '0' -&gt; Type</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>103</v>
       </c>
@@ -11461,7 +11463,7 @@
         <v>pxi_common.numb_format(tdu_net_weight, '9999999990.000', pxi_common.fc_is_nullable) || -- tdu_net_weight -&gt; ShipperNetWeightKG</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>99</v>
       </c>
@@ -11496,7 +11498,7 @@
         <v>pxi_common.numb_format(tdu_height, '9999999990', pxi_common.fc_is_nullable) || -- tdu_height -&gt; CaseHeight</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>98</v>
       </c>
@@ -11531,7 +11533,7 @@
         <v>pxi_common.numb_format(tdu_width, '9999999990', pxi_common.fc_is_nullable) || -- tdu_width -&gt; CaseWidth</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>97</v>
       </c>
@@ -11566,7 +11568,7 @@
         <v>pxi_common.numb_format(tdu_length, '9999999990', pxi_common.fc_is_nullable) || -- tdu_length -&gt; CaseLength</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>100</v>
       </c>
@@ -11601,7 +11603,7 @@
         <v>pxi_common.numb_format(rsu_height, '9999999990', pxi_common.fc_is_nullable) || -- rsu_height -&gt; UnitHeight</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>101</v>
       </c>
@@ -11636,7 +11638,7 @@
         <v>pxi_common.numb_format(rsu_width, '9999999990', pxi_common.fc_is_nullable) || -- rsu_width -&gt; UnitWidth</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>102</v>
       </c>
@@ -11678,7 +11680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -11691,7 +11693,7 @@
       <selection pane="bottomRight" activeCell="O2" sqref="O2:O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -11712,7 +11714,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -11751,7 +11753,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -11782,7 +11784,7 @@
         <v>pxi_common.char_format('303002', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '303002' -&gt; ICRecordType</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -11814,7 +11816,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -11846,7 +11848,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>131</v>
       </c>
@@ -11882,7 +11884,7 @@
         <v>pxi_common.char_format(node_code, 40, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- node_code -&gt; Attribute</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>132</v>
       </c>
@@ -11914,7 +11916,7 @@
         <v>pxi_common.char_format(node_name, 40, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- node_name -&gt; NodeName</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>133</v>
       </c>
@@ -11949,7 +11951,7 @@
         <v>pxi_common.char_format(parent_node_code, 40, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_nullable) || -- parent_node_code -&gt; ParrentAttribute</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>134</v>
       </c>
@@ -11984,51 +11986,51 @@
         <v>pxi_common.char_format(material_code, 18, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_nullable) || -- material_code -&gt; MaterialNumber</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M9" s="7" t="str">
         <f>IF(ISBLANK(H9),"",CONCATENATE(IF(LEN(H9)&lt;&gt;E9,"#",""),LEN(H9)))</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J10" s="10"/>
       <c r="M10" s="7" t="str">
         <f t="shared" ref="M10:M13" si="4">IF(ISBLANK(H10),"",CONCATENATE(IF(LEN(H10)&lt;&gt;E10,"#",""),LEN(H10)))</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M11" s="7" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M12" s="7" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="M13" s="7" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="10:15" ht="15">
+    <row r="22" spans="10:15" ht="15" x14ac:dyDescent="0.25">
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="10:15" ht="15">
+    <row r="23" spans="10:15" ht="15" x14ac:dyDescent="0.25">
       <c r="J23" s="10"/>
       <c r="O23" s="9"/>
     </row>
-    <row r="24" spans="10:15" ht="15">
+    <row r="24" spans="10:15" ht="15" x14ac:dyDescent="0.25">
       <c r="O24" s="9"/>
     </row>
-    <row r="25" spans="10:15" ht="15">
+    <row r="25" spans="10:15" ht="15" x14ac:dyDescent="0.25">
       <c r="O25" s="9"/>
     </row>
-    <row r="26" spans="10:15" ht="15">
+    <row r="26" spans="10:15" ht="15" x14ac:dyDescent="0.25">
       <c r="O26" s="9"/>
     </row>
   </sheetData>
@@ -12038,7 +12040,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -12051,7 +12053,7 @@
       <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -12072,7 +12074,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -12111,7 +12113,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>73</v>
       </c>
@@ -12142,7 +12144,7 @@
         <v>pxi_common.char_format('300001', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '300001' -&gt; RecordType</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
@@ -12174,7 +12176,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>29</v>
       </c>
@@ -12206,7 +12208,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
@@ -12241,7 +12243,7 @@
         <v>pxi_common.char_format(customer_code, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- customer_code -&gt; CustomerNumber</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -12273,7 +12275,7 @@
         <v>pxi_common.char_format(customer_name, 40, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- customer_name -&gt; Longname</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>48</v>
       </c>
@@ -12305,7 +12307,7 @@
         <v>pxi_common.char_format('Y', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT 'Y' -&gt; PACSCustomer</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>55</v>
       </c>
@@ -12340,7 +12342,7 @@
         <v>pxi_common.char_format(payer_customer_code, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_nullable) || -- payer_customer_code -&gt; PayerCode</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
@@ -12372,7 +12374,7 @@
         <v>pxi_common.char_format(tax_exempt, 1, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- tax_exempt -&gt; TaxExempt</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>50</v>
       </c>
@@ -12404,7 +12406,7 @@
         <v>pxi_common.char_format('NZD', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'NZD' -&gt; DefaultCurrenty</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>52</v>
       </c>
@@ -12436,7 +12438,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '149' -&gt; SalesOrg</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H12" s="3"/>
     </row>
   </sheetData>
@@ -12446,7 +12448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -12459,7 +12461,7 @@
       <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -12480,7 +12482,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -12519,7 +12521,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -12550,7 +12552,7 @@
         <v>pxi_common.char_format('301001', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '301001' -&gt; ICRecordType</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -12582,7 +12584,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -12614,7 +12616,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>159</v>
       </c>
@@ -12650,7 +12652,7 @@
         <v>pxi_common.char_format(cust_code, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- cust_code -&gt; CustomerNumber</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>160</v>
       </c>
@@ -12682,7 +12684,7 @@
         <v>pxi_common.char_format(cust_name, 40, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- cust_name -&gt; CustomerDescription</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>161</v>
       </c>
@@ -12714,7 +12716,7 @@
         <v>pxi_common.char_format(sales_org_code, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- sales_org_code -&gt; CustomerSalesOrg</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>162</v>
       </c>
@@ -12749,16 +12751,16 @@
         <v>pxi_common.char_format(parent_cust_code, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_nullable) || -- parent_cust_code -&gt; ParentCustomerNumber</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J9" s="10"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J10" s="10"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H12" s="3"/>
     </row>
   </sheetData>
@@ -12768,7 +12770,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -12781,7 +12783,7 @@
       <selection pane="bottomRight" activeCell="O2" sqref="O2:O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -12802,7 +12804,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -12841,7 +12843,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -12872,7 +12874,7 @@
         <v>pxi_common.char_format('347001', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '347001' -&gt; ICRecordType</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -12904,7 +12906,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -12936,7 +12938,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -12971,7 +12973,7 @@
         <v>pxi_common.char_format(company_code, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- company_code -&gt; VendorNumber</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
@@ -13003,7 +13005,7 @@
         <v>pxi_common.char_format(longname, 40, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- longname -&gt; Longname</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>44</v>
       </c>
@@ -13035,7 +13037,7 @@
         <v>pxi_common.char_format('Y', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT 'Y' -&gt; PACSVendor</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>45</v>
       </c>
@@ -13067,10 +13069,10 @@
         <v>pxi_common.char_format('1', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '1' -&gt; TaxExempt</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H12" s="3"/>
     </row>
   </sheetData>
@@ -13080,7 +13082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -13093,7 +13095,7 @@
       <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -13114,7 +13116,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -13153,7 +13155,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>73</v>
       </c>
@@ -13184,7 +13186,7 @@
         <v>pxi_common.char_format('330002', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '330002' -&gt; RecordType</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -13216,7 +13218,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -13248,7 +13250,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>115</v>
       </c>
@@ -13283,7 +13285,7 @@
         <v>pxi_common.char_format('DIV_1', 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- CONSTANT 'DIV_1' -&gt; CustomerCode</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>123</v>
       </c>
@@ -13315,7 +13317,7 @@
         <v>pxi_common.char_format(prodcode, 18, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- prodcode -&gt; MaterialCode</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>124</v>
       </c>
@@ -13348,7 +13350,7 @@
         <v>pxi_common.date_format(startdate, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- startdate -&gt; StartDate</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>125</v>
       </c>
@@ -13380,7 +13382,7 @@
         <v>pxi_common.date_format(enddate, 'yyyymmdd', pxi_common.fc_is_nullable) || -- enddate -&gt; EndDate</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>126</v>
       </c>
@@ -13412,7 +13414,7 @@
         <v>pxi_common.numb_format(listprice, '999999990.00', pxi_common.fc_is_nullable) || -- listprice -&gt; ListPrice</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>39</v>
       </c>
@@ -13444,10 +13446,10 @@
         <v>pxi_common.char_format('NZD', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'NZD' -&gt; Currency</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="J11" s="10"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H12" s="3"/>
     </row>
   </sheetData>
@@ -13457,20 +13459,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O38" sqref="O38"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -13491,7 +13493,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -13530,7 +13532,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -13561,7 +13563,7 @@
         <v>pxi_common.char_format('306001', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '306001' -&gt; ICRecordType</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -13596,7 +13598,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -13628,7 +13630,7 @@
         <v>pxi_common.char_format(hdr_division_code, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- hdr_division_code -&gt; PXDivisionCode</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -13663,7 +13665,7 @@
         <v>pxi_common.char_format(sold_to_cust_code, 20, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- sold_to_cust_code -&gt; CustomerNumber</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -13695,7 +13697,7 @@
         <v>pxi_common.char_format(billing_doc_num, 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- billing_doc_num -&gt; InvoiceNumber</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -13707,7 +13709,7 @@
         <v>42</v>
       </c>
       <c r="E7" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>2</v>
@@ -13724,10 +13726,10 @@
       </c>
       <c r="O7" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format(billing_doc_line_num, 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- billing_doc_line_num -&gt; InvoiceLineNumber</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+        <v>pxi_common.char_format(billing_doc_line_num, 10, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- billing_doc_line_num -&gt; InvoiceLineNumber</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -13736,7 +13738,7 @@
       </c>
       <c r="D8" s="8">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E8" s="1">
         <v>18</v>
@@ -13762,7 +13764,7 @@
         <v>pxi_common.char_format(matl_entd, 18, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- matl_entd -&gt; Material</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -13771,7 +13773,7 @@
       </c>
       <c r="D9" s="8">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E9" s="1">
         <v>8</v>
@@ -13797,7 +13799,7 @@
         <v>pxi_common.date_format(order_eff_date, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- order_eff_date -&gt; OrderDate</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -13806,7 +13808,7 @@
       </c>
       <c r="D10" s="8">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E10" s="1">
         <v>8</v>
@@ -13832,7 +13834,7 @@
         <v>pxi_common.date_format(billing_eff_date, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- billing_eff_date -&gt; InvoiceDate</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -13841,7 +13843,7 @@
       </c>
       <c r="D11" s="8">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E11" s="1">
         <v>17</v>
@@ -13867,7 +13869,7 @@
         <v>pxi_common.numb_format(billed_qty_base_uom, 'S9999999999990.00', pxi_common.fc_is_not_nullable) || -- billed_qty_base_uom -&gt; QuantityInvoiced</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -13876,7 +13878,7 @@
       </c>
       <c r="D12" s="8">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E12" s="1">
         <v>13</v>
@@ -13902,7 +13904,7 @@
         <v>pxi_common.numb_format(billed_gsv, 'S999999990.00', pxi_common.fc_is_not_nullable) || -- billed_gsv -&gt; GrossAmount</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -13911,7 +13913,7 @@
       </c>
       <c r="D13" s="8">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E13" s="1">
         <v>5</v>
@@ -13934,19 +13936,19 @@
         <v>pxi_common.char_format(doc_currcy_code, 5, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- doc_currcy_code -&gt; Currency</v>
       </c>
     </row>
-    <row r="22" spans="15:15" ht="15">
+    <row r="22" spans="15:15" ht="15" x14ac:dyDescent="0.25">
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="15:15" ht="15">
+    <row r="23" spans="15:15" ht="15" x14ac:dyDescent="0.25">
       <c r="O23" s="9"/>
     </row>
-    <row r="24" spans="15:15" ht="15">
+    <row r="24" spans="15:15" ht="15" x14ac:dyDescent="0.25">
       <c r="O24" s="9"/>
     </row>
-    <row r="25" spans="15:15" ht="15">
+    <row r="25" spans="15:15" ht="15" x14ac:dyDescent="0.25">
       <c r="O25" s="9"/>
     </row>
-    <row r="26" spans="15:15" ht="15">
+    <row r="26" spans="15:15" ht="15" x14ac:dyDescent="0.25">
       <c r="O26" s="9"/>
     </row>
   </sheetData>
@@ -13956,7 +13958,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -13969,7 +13971,7 @@
       <selection pane="bottomRight" activeCell="O2" sqref="O2:O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" style="1" customWidth="1"/>
@@ -13990,7 +13992,7 @@
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1">
+    <row r="1" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -14029,7 +14031,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -14060,7 +14062,7 @@
         <v>pxi_common.char_format('361001', 6, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '361001' -&gt; ICRecordType</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -14092,7 +14094,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -14124,7 +14126,7 @@
         <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>193</v>
       </c>
@@ -14159,7 +14161,7 @@
         <v>pxi_common.char_format(bus_partner_ref, 10, pxi_common.fc_format_type_ltrim_zeros, pxi_common.fc_is_not_nullable) || -- bus_partner_ref -&gt; AccountCode</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>191</v>
       </c>
@@ -14191,7 +14193,7 @@
         <v>pxi_common.char_format(tax_cust_ref, 20, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- tax_cust_ref -&gt; Reference</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>142</v>
       </c>
@@ -14223,7 +14225,7 @@
         <v>pxi_common.char_format('A', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT 'A' -&gt; ActionFlag</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
@@ -14255,7 +14257,7 @@
         <v>pxi_common.char_format('1', 1, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '1' -&gt; Type</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>152</v>
       </c>
@@ -14290,7 +14292,7 @@
         <v>pxi_common.date_format(posting_date, 'yyyymmdd', pxi_common.fc_is_not_nullable) || -- posting_date -&gt; Date</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>153</v>
       </c>
@@ -14322,7 +14324,7 @@
         <v>pxi_common.char_format(claim_ref, 18, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- claim_ref -&gt; Number</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>144</v>
       </c>
@@ -14355,7 +14357,7 @@
         <v>pxi_common.char_format('0', 18, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '0' -&gt; ParentNumber</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>150</v>
       </c>
@@ -14388,7 +14390,7 @@
         <v>pxi_common.char_format(assignment_no, 65, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- assignment_no -&gt; ExtReference</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C13" s="1" t="s">
         <v>146</v>
       </c>
@@ -14420,7 +14422,7 @@
         <v>pxi_common.char_format('', 80, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '' -&gt; InvoiceLink</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>154</v>
       </c>
@@ -14452,7 +14454,7 @@
         <v>pxi_common.char_format(reason_code, 5, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- reason_code -&gt; ReasonCode</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>190</v>
       </c>
@@ -14487,7 +14489,7 @@
         <v>pxi_common.numb_format(amount, '9999999990.00', pxi_common.fc_is_not_nullable) || -- amount -&gt; Amount</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>192</v>
       </c>
@@ -14522,7 +14524,7 @@
         <v>pxi_common.numb_format(tax_amount, '9999999990.00', pxi_common.fc_is_not_nullable) || -- tax_amount -&gt; TaxAmount</v>
       </c>
     </row>
-    <row r="17" spans="3:15">
+    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
         <v>149</v>
       </c>
@@ -14554,7 +14556,7 @@
         <v>pxi_common.char_format('', 256, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '' -&gt; Note</v>
       </c>
     </row>
-    <row r="18" spans="3:15">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Flag buy_stop_date as required
</commit_message>
<xml_diff>
--- a/SOURCE/PXI/DOC/Promax Interface Format 20130802_3.xlsx
+++ b/SOURCE/PXI/DOC/Promax Interface Format 20130802_3.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20730" windowHeight="4245" tabRatio="635" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20730" windowHeight="4245" tabRatio="635" firstSheet="12" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Interface Master" sheetId="14" r:id="rId1"/>
@@ -1777,6 +1777,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2607,7 +2608,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet10">
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O11"/>
@@ -3021,7 +3022,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet11">
     <tabColor theme="6" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3696,7 +3697,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet12">
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:N35"/>
@@ -4938,7 +4939,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet13">
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:N35"/>
@@ -6702,7 +6703,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet14">
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:N40"/>
@@ -8753,17 +8754,17 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet15">
     <tabColor theme="8" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9229,7 +9230,7 @@
         <v>8</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>3</v>
@@ -9250,7 +9251,7 @@
       </c>
       <c r="L9" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>fflu_data.add_date_field_txt(pc_buy_stop_date,59,8,'yyyymmdd',fflu_data.gc_null_min_date,fflu_data.gc_null_max_date,fflu_data.gc_allow_null,fflu_data.gc_null_nls_options);</v>
+        <v>fflu_data.add_date_field_txt(pc_buy_stop_date,59,8,'yyyymmdd',fflu_data.gc_null_min_date,fflu_data.gc_null_max_date,fflu_data.gc_not_allow_null,fflu_data.gc_null_nls_options);</v>
       </c>
       <c r="M9" s="8" t="str">
         <f t="shared" ca="1" si="6"/>
@@ -10731,7 +10732,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet16">
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B24"/>
@@ -10893,7 +10894,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet2">
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O22"/>
@@ -11681,7 +11682,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet3">
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O26"/>
@@ -12041,7 +12042,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet4">
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O12"/>
@@ -12449,7 +12450,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet5">
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O12"/>
@@ -12771,7 +12772,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet6">
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O12"/>
@@ -13083,7 +13084,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet7">
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O12"/>
@@ -13460,12 +13461,12 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet8">
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -13959,7 +13960,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr codeName="Sheet9">
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:O18"/>

</xml_diff>

<commit_message>
Removed the old version I had created and applied the promax company and division information into the current master copy.
</commit_message>
<xml_diff>
--- a/SOURCE/PXI/DOC/Promax Interface Format 20130802_3.xlsx
+++ b/SOURCE/PXI/DOC/Promax Interface Format 20130802_3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20730" windowHeight="4245" tabRatio="635" firstSheet="12" activeTab="14"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="25230" windowHeight="6480" tabRatio="635" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Interface Master" sheetId="14" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1567" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="448">
   <si>
     <t>No</t>
   </si>
@@ -1383,6 +1383,12 @@
   </si>
   <si>
     <t>product_status</t>
+  </si>
+  <si>
+    <t>promax_company</t>
+  </si>
+  <si>
+    <t>promax_division</t>
   </si>
 </sst>
 </file>
@@ -2617,7 +2623,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2712,6 +2718,9 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>446</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -2729,26 +2738,27 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J3" s="10"/>
       <c r="M3" s="7" t="str">
         <f t="shared" ref="M3:M11" si="1">IF(ISBLANK(H3),"",CONCATENATE(IF(LEN(H3)&lt;&gt;E3,"#",""),LEN(H3)))</f>
         <v/>
       </c>
       <c r="O3" s="8" t="str">
         <f t="shared" ref="O3:O11" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+        <v>pxi_common.char_format(promax_company, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_company -&gt; PXCompanyCode</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" ref="D4:D10" si="3">D3+E3</f>
+        <f t="shared" ref="D4" si="3">D3+E3</f>
         <v>9</v>
       </c>
       <c r="E4" s="1">
@@ -2761,18 +2771,16 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J4" s="10"/>
       <c r="M4" s="7" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="O4" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+        <v>pxi_common.char_format(promax_division, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_division -&gt; PXDivisionCode</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -2783,7 +2791,7 @@
         <v>32</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D4:D10" si="4">D4+E4</f>
         <v>12</v>
       </c>
       <c r="E5" s="1">
@@ -2815,7 +2823,7 @@
         <v>33</v>
       </c>
       <c r="D6" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="E6" s="1">
@@ -2847,7 +2855,7 @@
         <v>166</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
       <c r="E7" s="1">
@@ -2883,7 +2891,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="E8" s="1">
@@ -2919,7 +2927,7 @@
         <v>36</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="E9" s="1">
@@ -2954,7 +2962,7 @@
         <v>167</v>
       </c>
       <c r="D10" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="E10" s="1">
@@ -3028,8 +3036,8 @@
   </sheetPr>
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -6712,7 +6720,7 @@
       <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8760,11 +8768,11 @@
   </sheetPr>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="10" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10903,7 +10911,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -10998,11 +11006,14 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>446</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3:D22" si="1">D2+E2</f>
+        <f t="shared" ref="D3:D4" si="1">D2+E2</f>
         <v>6</v>
       </c>
       <c r="E3" s="1">
@@ -11014,23 +11025,23 @@
       <c r="G3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="3"/>
       <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J3" s="10"/>
       <c r="M3" s="7" t="str">
         <f>IF(ISBLANK(H3),"",CONCATENATE(IF(LEN(H3)&lt;&gt;E3,"#",""),LEN(H3)))</f>
         <v/>
       </c>
       <c r="O3" s="8" t="str">
         <f t="shared" ref="O3:O22" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+        <v>pxi_common.char_format(promax_company, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_company -&gt; PXCompanyCode</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -11047,20 +11058,17 @@
       <c r="G4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="3"/>
       <c r="I4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J4" s="10"/>
       <c r="M4" s="7" t="str">
         <f>IF(ISBLANK(H4),"",CONCATENATE(IF(LEN(H4)&lt;&gt;E4,"#",""),LEN(H4)))</f>
         <v/>
       </c>
       <c r="O4" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+        <v>pxi_common.char_format(promax_division, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_division -&gt; PXDivisionCode</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -11071,7 +11079,7 @@
         <v>74</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D3:D22" si="3">D4+E4</f>
         <v>12</v>
       </c>
       <c r="E5" s="1">
@@ -11090,7 +11098,7 @@
         <v>64</v>
       </c>
       <c r="M5" s="7" t="str">
-        <f t="shared" ref="M5:M20" si="3">IF(ISBLANK(H5),"",CONCATENATE(IF(LEN(H5)&lt;&gt;E5,"#",""),LEN(H5)))</f>
+        <f t="shared" ref="M5:M20" si="4">IF(ISBLANK(H5),"",CONCATENATE(IF(LEN(H5)&lt;&gt;E5,"#",""),LEN(H5)))</f>
         <v/>
       </c>
       <c r="O5" s="8" t="str">
@@ -11106,7 +11114,7 @@
         <v>109</v>
       </c>
       <c r="D6" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="E6" s="1">
@@ -11122,7 +11130,7 @@
         <v>0</v>
       </c>
       <c r="M6" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O6" s="8" t="str">
@@ -11138,7 +11146,7 @@
         <v>75</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="E7" s="1">
@@ -11155,7 +11163,7 @@
       </c>
       <c r="J7" s="10"/>
       <c r="M7" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O7" s="8" t="str">
@@ -11171,7 +11179,7 @@
         <v>76</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
       <c r="E8" s="1">
@@ -11190,7 +11198,7 @@
         <v>64</v>
       </c>
       <c r="M8" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O8" s="8" t="str">
@@ -11206,7 +11214,7 @@
         <v>77</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
       <c r="E9" s="1">
@@ -11222,7 +11230,7 @@
         <v>0</v>
       </c>
       <c r="M9" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O9" s="8" t="str">
@@ -11238,7 +11246,7 @@
         <v>78</v>
       </c>
       <c r="D10" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="E10" s="1">
@@ -11254,7 +11262,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O10" s="8" t="str">
@@ -11270,7 +11278,7 @@
         <v>79</v>
       </c>
       <c r="D11" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>118</v>
       </c>
       <c r="E11" s="1">
@@ -11286,7 +11294,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O11" s="8" t="str">
@@ -11302,7 +11310,7 @@
         <v>111</v>
       </c>
       <c r="D12" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>121</v>
       </c>
       <c r="E12" s="1">
@@ -11319,7 +11327,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O12" s="8" t="str">
@@ -11335,7 +11343,7 @@
         <v>80</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>124</v>
       </c>
       <c r="E13" s="1">
@@ -11354,7 +11362,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="O13" s="8" t="str">
@@ -11370,7 +11378,7 @@
         <v>82</v>
       </c>
       <c r="D14" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>138</v>
       </c>
       <c r="E14" s="1">
@@ -11389,7 +11397,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="O14" s="8" t="str">
@@ -11402,7 +11410,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>152</v>
       </c>
       <c r="E15" s="1">
@@ -11421,7 +11429,7 @@
         <v>108</v>
       </c>
       <c r="M15" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O15" s="8" t="str">
@@ -11437,7 +11445,7 @@
         <v>83</v>
       </c>
       <c r="D16" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>153</v>
       </c>
       <c r="E16" s="1">
@@ -11456,7 +11464,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="O16" s="8" t="str">
@@ -11472,7 +11480,7 @@
         <v>85</v>
       </c>
       <c r="D17" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>167</v>
       </c>
       <c r="E17" s="1">
@@ -11491,7 +11499,7 @@
         <v>0</v>
       </c>
       <c r="M17" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="O17" s="8" t="str">
@@ -11507,7 +11515,7 @@
         <v>86</v>
       </c>
       <c r="D18" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>177</v>
       </c>
       <c r="E18" s="1">
@@ -11526,7 +11534,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="O18" s="8" t="str">
@@ -11542,7 +11550,7 @@
         <v>87</v>
       </c>
       <c r="D19" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>187</v>
       </c>
       <c r="E19" s="1">
@@ -11561,7 +11569,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="O19" s="8" t="str">
@@ -11577,7 +11585,7 @@
         <v>88</v>
       </c>
       <c r="D20" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>197</v>
       </c>
       <c r="E20" s="1">
@@ -11596,7 +11604,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="O20" s="8" t="str">
@@ -11612,7 +11620,7 @@
         <v>89</v>
       </c>
       <c r="D21" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>207</v>
       </c>
       <c r="E21" s="1">
@@ -11631,7 +11639,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="7" t="str">
-        <f t="shared" ref="M21:M22" si="4">IF(ISBLANK(H21),"",CONCATENATE(IF(LEN(H21)&lt;&gt;E21,"#",""),LEN(H21)))</f>
+        <f t="shared" ref="M21:M22" si="5">IF(ISBLANK(H21),"",CONCATENATE(IF(LEN(H21)&lt;&gt;E21,"#",""),LEN(H21)))</f>
         <v>10</v>
       </c>
       <c r="O21" s="8" t="str">
@@ -11647,7 +11655,7 @@
         <v>90</v>
       </c>
       <c r="D22" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>217</v>
       </c>
       <c r="E22" s="1">
@@ -11666,7 +11674,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="O22" s="8" t="str">
@@ -11691,7 +11699,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2:O8"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="A3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -12051,7 +12059,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -12146,11 +12154,14 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>446</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3:D11" si="1">D2+E2</f>
+        <f t="shared" ref="D3:D4" si="1">D2+E2</f>
         <v>6</v>
       </c>
       <c r="E3" s="1">
@@ -12163,23 +12174,24 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J3" s="10"/>
       <c r="M3" s="7" t="str">
         <f t="shared" ref="M3:M4" si="2">IF(ISBLANK(H3),"",CONCATENATE(IF(LEN(H3)&lt;&gt;E3,"#",""),LEN(H3)))</f>
         <v/>
       </c>
       <c r="O3" s="8" t="str">
         <f t="shared" ref="O3:O11" ca="1" si="3">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+        <v>pxi_common.char_format(promax_company, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_company -&gt; PXCompanyCode</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" si="1"/>
@@ -12195,18 +12207,16 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J4" s="10"/>
       <c r="M4" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="O4" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+        <v>pxi_common.char_format(promax_division, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_division -&gt; PXDivisionCode</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -12217,7 +12227,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D3:D11" si="4">D4+E4</f>
         <v>12</v>
       </c>
       <c r="E5" s="1">
@@ -12252,7 +12262,7 @@
         <v>43</v>
       </c>
       <c r="D6" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="E6" s="1">
@@ -12281,7 +12291,7 @@
         <v>48</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="E7" s="1">
@@ -12316,7 +12326,7 @@
         <v>49</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>63</v>
       </c>
       <c r="E8" s="1">
@@ -12351,7 +12361,7 @@
         <v>45</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>73</v>
       </c>
       <c r="E9" s="1">
@@ -12380,7 +12390,7 @@
         <v>50</v>
       </c>
       <c r="D10" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>74</v>
       </c>
       <c r="E10" s="1">
@@ -12412,7 +12422,7 @@
         <v>52</v>
       </c>
       <c r="D11" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>77</v>
       </c>
       <c r="E11" s="1">
@@ -12459,7 +12469,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -12554,6 +12564,9 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>446</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
@@ -12571,26 +12584,27 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J3" s="10"/>
       <c r="M3" s="7" t="str">
         <f t="shared" ref="M3:M8" si="1">IF(ISBLANK(H3),"",CONCATENATE(IF(LEN(H3)&lt;&gt;E3,"#",""),LEN(H3)))</f>
         <v/>
       </c>
       <c r="O3" s="8" t="str">
         <f t="shared" ref="O3:O8" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+        <v>pxi_common.char_format(promax_company, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_company -&gt; PXCompanyCode</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" ref="D4:D8" si="3">D3+E3</f>
+        <f t="shared" ref="D4" si="3">D3+E3</f>
         <v>9</v>
       </c>
       <c r="E4" s="1">
@@ -12603,18 +12617,16 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J4" s="10"/>
       <c r="M4" s="7" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="O4" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+        <v>pxi_common.char_format(promax_division, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_division -&gt; PXDivisionCode</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -12625,7 +12637,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D4:D8" si="4">D4+E4</f>
         <v>12</v>
       </c>
       <c r="E5" s="1">
@@ -12661,7 +12673,7 @@
         <v>156</v>
       </c>
       <c r="D6" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="E6" s="1">
@@ -12693,7 +12705,7 @@
         <v>157</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>62</v>
       </c>
       <c r="E7" s="1">
@@ -12725,7 +12737,7 @@
         <v>158</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="E8" s="1">
@@ -12781,7 +12793,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2:O8"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -12876,11 +12888,14 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>446</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3" si="1">D2+E2</f>
+        <f t="shared" ref="D3:D4" si="1">D2+E2</f>
         <v>6</v>
       </c>
       <c r="E3" s="1">
@@ -12893,26 +12908,27 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J3" s="10"/>
       <c r="M3" s="7" t="str">
         <f>IF(ISBLANK(H3),"",CONCATENATE(IF(LEN(H3)&lt;&gt;E3,"#",""),LEN(H3)))</f>
         <v/>
       </c>
       <c r="O3" s="8" t="str">
         <f t="shared" ref="O3:O8" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+        <v>pxi_common.char_format(promax_company, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_company -&gt; PXCompanyCode</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" ref="D4:D8" si="3">D3+E3</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E4" s="1">
@@ -12925,18 +12941,16 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J4" s="10"/>
       <c r="M4" s="7" t="str">
         <f>IF(ISBLANK(H4),"",CONCATENATE(IF(LEN(H4)&lt;&gt;E4,"#",""),LEN(H4)))</f>
         <v/>
       </c>
       <c r="O4" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+        <v>pxi_common.char_format(promax_division, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_division -&gt; PXDivisionCode</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -12947,7 +12961,7 @@
         <v>42</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D4:D8" si="3">D4+E4</f>
         <v>12</v>
       </c>
       <c r="E5" s="1">
@@ -13093,7 +13107,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O11" sqref="O11"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -13188,11 +13202,14 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>446</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3" si="1">D2+E2</f>
+        <f t="shared" ref="D3:D4" si="1">D2+E2</f>
         <v>6</v>
       </c>
       <c r="E3" s="1">
@@ -13205,26 +13222,27 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J3" s="10"/>
       <c r="M3" s="7" t="str">
         <f>IF(ISBLANK(H3),"",CONCATENATE(IF(LEN(H3)&lt;&gt;E3,"#",""),LEN(H3)))</f>
         <v/>
       </c>
       <c r="O3" s="8" t="str">
         <f t="shared" ref="O3:O10" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+        <v>pxi_common.char_format(promax_company, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- promax_company -&gt; PXCompanyCode</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" ref="D4:D10" si="3">D3+E3</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="E4" s="1">
@@ -13237,18 +13255,16 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J4" s="10"/>
       <c r="M4" s="7" t="str">
         <f>IF(ISBLANK(H4),"",CONCATENATE(IF(LEN(H4)&lt;&gt;E4,"#",""),LEN(H4)))</f>
         <v/>
       </c>
       <c r="O4" s="8" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+        <v>pxi_common.char_format(promax_division, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_nullable) || -- promax_division -&gt; PXDivisionCode</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -13256,7 +13272,7 @@
         <v>115</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D4:D10" si="3">D4+E4</f>
         <v>12</v>
       </c>
       <c r="E5" s="1">
@@ -13470,7 +13486,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -13572,7 +13588,7 @@
         <v>29</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3:D13" si="1">D2+E2</f>
+        <f t="shared" ref="D3" si="1">D2+E2</f>
         <v>6</v>
       </c>
       <c r="E3" s="1">
@@ -13585,18 +13601,16 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J3" s="10"/>
       <c r="M3" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="O3" s="8" t="str">
         <f t="shared" ref="O3:O13" ca="1" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+        <v>pxi_common.char_format(company_code, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- company_code -&gt; PXCompanyCode</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -13607,7 +13621,7 @@
         <v>30</v>
       </c>
       <c r="D4" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D3:D13" si="3">D3+E3</f>
         <v>9</v>
       </c>
       <c r="E4" s="1">
@@ -13639,7 +13653,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="E5" s="1">
@@ -13674,7 +13688,7 @@
         <v>32</v>
       </c>
       <c r="D6" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="E6" s="1">
@@ -13706,7 +13720,7 @@
         <v>33</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="E7" s="1">
@@ -13738,7 +13752,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="E8" s="1">
@@ -13773,7 +13787,7 @@
         <v>35</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="E9" s="1">
@@ -13808,7 +13822,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>78</v>
       </c>
       <c r="E10" s="1">
@@ -13827,7 +13841,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="7" t="str">
-        <f t="shared" ref="M10:M13" si="3">IF(ISBLANK(H10),"",CONCATENATE(IF(LEN(H10)&lt;&gt;E10,"#",""),LEN(H10)))</f>
+        <f t="shared" ref="M10:M13" si="4">IF(ISBLANK(H10),"",CONCATENATE(IF(LEN(H10)&lt;&gt;E10,"#",""),LEN(H10)))</f>
         <v>8</v>
       </c>
       <c r="O10" s="8" t="str">
@@ -13843,7 +13857,7 @@
         <v>37</v>
       </c>
       <c r="D11" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
       <c r="E11" s="1">
@@ -13862,7 +13876,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="O11" s="8" t="str">
@@ -13878,7 +13892,7 @@
         <v>38</v>
       </c>
       <c r="D12" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>103</v>
       </c>
       <c r="E12" s="1">
@@ -13897,7 +13911,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="O12" s="8" t="str">
@@ -13913,7 +13927,7 @@
         <v>39</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>116</v>
       </c>
       <c r="E13" s="1">
@@ -13929,7 +13943,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O13" s="8" t="str">
@@ -13969,7 +13983,7 @@
       <pane xSplit="12" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2:O18"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -14064,11 +14078,14 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>446</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D3" s="8">
-        <f t="shared" ref="D3:D18" si="1">D2+E2</f>
+        <f t="shared" ref="D3:D4" si="1">D2+E2</f>
         <v>6</v>
       </c>
       <c r="E3" s="1">
@@ -14081,21 +14098,22 @@
         <v>1</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J3" s="10"/>
       <c r="M3" s="7" t="str">
         <f t="shared" ref="M3:M18" si="2">IF(ISBLANK(H3),"",CONCATENATE(IF(LEN(H3)&lt;&gt;E3,"#",""),LEN(H3)))</f>
         <v/>
       </c>
       <c r="O3" s="8" t="str">
         <f t="shared" ref="O3:O18" ca="1" si="3">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDIRECT(UPPER(CONCATENATE(G3,IF(I3="Yes","_CONSTANT","")))), "::source_field::", A3), "::target_field::", C3), "::position::", D3), "::length::", E3), "::format::", H3), "::constant::", J3), "::is_nullable::", IF(F3="Yes", "pxi_common.fc_is_not_nullable", "pxi_common.fc_is_nullable")), "::format_type::", CONCATENATE("pxi_common.fc_format_type_", IF(ISBLANK(L3), "none", LOWER(L3))))</f>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXCompanyCode</v>
+        <v>pxi_common.char_format(promax_company, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_company -&gt; PXCompanyCode</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>30</v>
       </c>
@@ -14113,18 +14131,16 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>107</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J4" s="10"/>
       <c r="M4" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="O4" s="8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>pxi_common.char_format('149', 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- CONSTANT '149' -&gt; PXDivisionCode</v>
+        <v>pxi_common.char_format(promax_division, 3, pxi_common.fc_format_type_none, pxi_common.fc_is_not_nullable) || -- promax_division -&gt; PXDivisionCode</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -14135,7 +14151,7 @@
         <v>140</v>
       </c>
       <c r="D5" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D3:D18" si="4">D4+E4</f>
         <v>12</v>
       </c>
       <c r="E5" s="1">
@@ -14170,7 +14186,7 @@
         <v>141</v>
       </c>
       <c r="D6" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>22</v>
       </c>
       <c r="E6" s="1">
@@ -14199,7 +14215,7 @@
         <v>142</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>42</v>
       </c>
       <c r="E7" s="1">
@@ -14231,7 +14247,7 @@
         <v>8</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="E8" s="1">
@@ -14266,7 +14282,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>44</v>
       </c>
       <c r="E9" s="1">
@@ -14301,7 +14317,7 @@
         <v>143</v>
       </c>
       <c r="D10" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="E10" s="1">
@@ -14330,7 +14346,7 @@
         <v>144</v>
       </c>
       <c r="D11" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="E11" s="1">
@@ -14366,7 +14382,7 @@
         <v>145</v>
       </c>
       <c r="D12" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>88</v>
       </c>
       <c r="E12" s="1">
@@ -14396,7 +14412,7 @@
         <v>146</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>153</v>
       </c>
       <c r="E13" s="1">
@@ -14431,7 +14447,7 @@
         <v>147</v>
       </c>
       <c r="D14" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>233</v>
       </c>
       <c r="E14" s="1">
@@ -14463,7 +14479,7 @@
         <v>148</v>
       </c>
       <c r="D15" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>238</v>
       </c>
       <c r="E15" s="1">
@@ -14498,7 +14514,7 @@
         <v>136</v>
       </c>
       <c r="D16" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>251</v>
       </c>
       <c r="E16" s="1">
@@ -14530,7 +14546,7 @@
         <v>149</v>
       </c>
       <c r="D17" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>264</v>
       </c>
       <c r="E17" s="1">
@@ -14562,7 +14578,7 @@
         <v>39</v>
       </c>
       <c r="D18" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>520</v>
       </c>
       <c r="E18" s="1">

</xml_diff>